<commit_message>
fouten opgelost in origineel xlsx bestand
</commit_message>
<xml_diff>
--- a/src/main/resources/nhs-dmn/CHgestript.xlsx
+++ b/src/main/resources/nhs-dmn/CHgestript.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-20.04\home\han\git\rivm\nhs\dmn\nhs-business\src\main\resources\nhs-dmn\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD7E9058-EDAB-4DB3-ADEC-0907F5CAA343}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{270E6B09-B1AC-4C35-AB73-29D9E107077C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="834" xr2:uid="{4203C9A5-FA6C-4E14-8325-EE7186AD0D41}"/>
   </bookViews>
@@ -126,6 +126,15 @@
     <t>false</t>
   </si>
   <si>
+    <t>"Afwijkend"</t>
+  </si>
+  <si>
+    <t>"Dubieus"</t>
+  </si>
+  <si>
+    <t>"Negatief"</t>
+  </si>
+  <si>
     <t>(-3.0 .. -1.6]</t>
   </si>
   <si>
@@ -147,21 +156,12 @@
     <t>afname - geboorte</t>
   </si>
   <si>
-    <t>Ja</t>
-  </si>
-  <si>
-    <t>ja</t>
-  </si>
-  <si>
     <t>&gt;= 48</t>
   </si>
   <si>
     <t>AfnameTijd EN GeboorteTijd bekend?</t>
   </si>
   <si>
-    <t>Nee</t>
-  </si>
-  <si>
     <t>&gt;= 72</t>
   </si>
   <si>
@@ -171,15 +171,6 @@
     <t>MeetResultaat</t>
   </si>
   <si>
-    <t>Afwijkend</t>
-  </si>
-  <si>
-    <t>Dubieus</t>
-  </si>
-  <si>
-    <t>Negatief</t>
-  </si>
-  <si>
     <t>THP</t>
   </si>
   <si>
@@ -190,6 +181,15 @@
   </si>
   <si>
     <t>hielprik.hielprikType</t>
+  </si>
+  <si>
+    <t>onbekend(hielprik,"T4")</t>
+  </si>
+  <si>
+    <t>onbekend(hielprik,"TSH")</t>
+  </si>
+  <si>
+    <t>onbekend(hielprik,"T4/TBG")</t>
   </si>
 </sst>
 </file>
@@ -673,12 +673,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{920955FF-C75C-492B-A53F-AFC4A746FDCE}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:G82"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K25" sqref="K25"/>
+      <selection pane="bottomLeft" activeCell="H1" sqref="H1:H1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -688,7 +687,7 @@
     <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -696,7 +695,7 @@
         <v>15</v>
       </c>
       <c r="B1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
@@ -714,7 +713,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>22</v>
       </c>
@@ -722,22 +721,22 @@
         <v>22</v>
       </c>
       <c r="C2" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="D2" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="E2" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="F2" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="G2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -745,22 +744,22 @@
         <v>22</v>
       </c>
       <c r="C3" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="D3" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="E3" t="s">
         <v>19</v>
       </c>
       <c r="F3" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="G3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -768,22 +767,22 @@
         <v>22</v>
       </c>
       <c r="C4" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="D4" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="E4" t="s">
         <v>13</v>
       </c>
       <c r="F4" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="G4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -791,22 +790,22 @@
         <v>22</v>
       </c>
       <c r="C5" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="D5" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="E5" t="s">
         <v>12</v>
       </c>
       <c r="F5" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="G5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>23</v>
       </c>
@@ -814,22 +813,22 @@
         <v>23</v>
       </c>
       <c r="C6" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="D6" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="E6" t="s">
+        <v>28</v>
+      </c>
+      <c r="F6" t="s">
+        <v>30</v>
+      </c>
+      <c r="G6" t="s">
         <v>25</v>
       </c>
-      <c r="F6" t="s">
-        <v>27</v>
-      </c>
-      <c r="G6" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>23</v>
       </c>
@@ -837,45 +836,45 @@
         <v>22</v>
       </c>
       <c r="C7" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="D7" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="E7" t="s">
+        <v>28</v>
+      </c>
+      <c r="F7" t="s">
+        <v>30</v>
+      </c>
+      <c r="G7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" t="s">
+        <v>30</v>
+      </c>
+      <c r="E8" t="s">
+        <v>28</v>
+      </c>
+      <c r="F8" t="s">
+        <v>30</v>
+      </c>
+      <c r="G8" t="s">
         <v>25</v>
       </c>
-      <c r="F7" t="s">
-        <v>27</v>
-      </c>
-      <c r="G7" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>22</v>
-      </c>
-      <c r="B8" t="s">
-        <v>23</v>
-      </c>
-      <c r="C8" t="s">
-        <v>26</v>
-      </c>
-      <c r="D8" t="s">
-        <v>27</v>
-      </c>
-      <c r="E8" t="s">
-        <v>25</v>
-      </c>
-      <c r="F8" t="s">
-        <v>27</v>
-      </c>
-      <c r="G8" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>23</v>
       </c>
@@ -883,22 +882,22 @@
         <v>23</v>
       </c>
       <c r="C9" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="D9" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="E9" t="s">
         <v>19</v>
       </c>
       <c r="F9" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="G9" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>23</v>
       </c>
@@ -906,22 +905,22 @@
         <v>22</v>
       </c>
       <c r="C10" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="D10" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="E10" t="s">
         <v>19</v>
       </c>
       <c r="F10" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="G10" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>22</v>
       </c>
@@ -929,22 +928,22 @@
         <v>23</v>
       </c>
       <c r="C11" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="D11" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="E11" t="s">
         <v>19</v>
       </c>
       <c r="F11" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="G11" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>23</v>
       </c>
@@ -952,22 +951,22 @@
         <v>23</v>
       </c>
       <c r="C12" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="D12" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="E12" t="s">
         <v>13</v>
       </c>
       <c r="F12" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="G12" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>23</v>
       </c>
@@ -975,22 +974,22 @@
         <v>22</v>
       </c>
       <c r="C13" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="D13" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="E13" t="s">
         <v>13</v>
       </c>
       <c r="F13" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="G13" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>22</v>
       </c>
@@ -998,22 +997,22 @@
         <v>23</v>
       </c>
       <c r="C14" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="D14" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="E14" t="s">
         <v>13</v>
       </c>
       <c r="F14" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="G14" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>23</v>
       </c>
@@ -1021,22 +1020,22 @@
         <v>23</v>
       </c>
       <c r="C15" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="D15" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="E15" t="s">
         <v>12</v>
       </c>
       <c r="F15" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="G15" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>23</v>
       </c>
@@ -1044,22 +1043,22 @@
         <v>22</v>
       </c>
       <c r="C16" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="D16" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="E16" t="s">
         <v>12</v>
       </c>
       <c r="F16" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="G16" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>22</v>
       </c>
@@ -1067,19 +1066,19 @@
         <v>23</v>
       </c>
       <c r="C17" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="D17" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="E17" t="s">
         <v>12</v>
       </c>
       <c r="F17" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="G17" t="s">
-        <v>12</v>
+        <v>44</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -1090,19 +1089,19 @@
         <v>23</v>
       </c>
       <c r="C18" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D18" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="E18" t="s">
+        <v>28</v>
+      </c>
+      <c r="F18" t="s">
+        <v>30</v>
+      </c>
+      <c r="G18" t="s">
         <v>25</v>
-      </c>
-      <c r="F18" t="s">
-        <v>27</v>
-      </c>
-      <c r="G18" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -1113,19 +1112,19 @@
         <v>23</v>
       </c>
       <c r="C19" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D19" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="E19" t="s">
+        <v>28</v>
+      </c>
+      <c r="F19" t="s">
+        <v>30</v>
+      </c>
+      <c r="G19" t="s">
         <v>25</v>
-      </c>
-      <c r="F19" t="s">
-        <v>27</v>
-      </c>
-      <c r="G19" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -1136,19 +1135,19 @@
         <v>22</v>
       </c>
       <c r="C20" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D20" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="E20" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="F20" t="s">
         <v>20</v>
       </c>
       <c r="G20" t="s">
-        <v>39</v>
+        <v>24</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -1159,19 +1158,19 @@
         <v>22</v>
       </c>
       <c r="C21" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D21" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="E21" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="F21" t="s">
         <v>21</v>
       </c>
       <c r="G21" t="s">
-        <v>39</v>
+        <v>24</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -1182,19 +1181,19 @@
         <v>22</v>
       </c>
       <c r="C22" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D22" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="E22" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="F22" t="s">
         <v>12</v>
       </c>
       <c r="G22" t="s">
-        <v>39</v>
+        <v>24</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
@@ -1205,10 +1204,10 @@
         <v>23</v>
       </c>
       <c r="C23" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D23" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="E23" t="s">
         <v>19</v>
@@ -1217,7 +1216,7 @@
         <v>20</v>
       </c>
       <c r="G23" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -1228,10 +1227,10 @@
         <v>22</v>
       </c>
       <c r="C24" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D24" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="E24" t="s">
         <v>19</v>
@@ -1240,7 +1239,7 @@
         <v>20</v>
       </c>
       <c r="G24" t="s">
-        <v>39</v>
+        <v>24</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
@@ -1251,10 +1250,10 @@
         <v>23</v>
       </c>
       <c r="C25" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D25" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="E25" t="s">
         <v>19</v>
@@ -1263,7 +1262,7 @@
         <v>20</v>
       </c>
       <c r="G25" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
@@ -1274,10 +1273,10 @@
         <v>23</v>
       </c>
       <c r="C26" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D26" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="E26" t="s">
         <v>19</v>
@@ -1286,7 +1285,7 @@
         <v>21</v>
       </c>
       <c r="G26" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
@@ -1297,10 +1296,10 @@
         <v>22</v>
       </c>
       <c r="C27" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D27" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="E27" t="s">
         <v>19</v>
@@ -1309,7 +1308,7 @@
         <v>21</v>
       </c>
       <c r="G27" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
@@ -1320,10 +1319,10 @@
         <v>23</v>
       </c>
       <c r="C28" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D28" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="E28" t="s">
         <v>19</v>
@@ -1332,7 +1331,7 @@
         <v>21</v>
       </c>
       <c r="G28" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
@@ -1343,10 +1342,10 @@
         <v>23</v>
       </c>
       <c r="C29" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D29" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="E29" t="s">
         <v>19</v>
@@ -1355,7 +1354,7 @@
         <v>12</v>
       </c>
       <c r="G29" t="s">
-        <v>12</v>
+        <v>45</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
@@ -1366,10 +1365,10 @@
         <v>22</v>
       </c>
       <c r="C30" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D30" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="E30" t="s">
         <v>19</v>
@@ -1378,7 +1377,7 @@
         <v>12</v>
       </c>
       <c r="G30" t="s">
-        <v>12</v>
+        <v>45</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
@@ -1389,10 +1388,10 @@
         <v>23</v>
       </c>
       <c r="C31" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D31" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="E31" t="s">
         <v>19</v>
@@ -1401,7 +1400,7 @@
         <v>12</v>
       </c>
       <c r="G31" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
@@ -1412,19 +1411,19 @@
         <v>23</v>
       </c>
       <c r="C32" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D32" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="E32" t="s">
         <v>13</v>
       </c>
       <c r="F32" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="G32" t="s">
-        <v>39</v>
+        <v>24</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
@@ -1435,19 +1434,19 @@
         <v>23</v>
       </c>
       <c r="C33" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D33" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="E33" t="s">
         <v>13</v>
       </c>
       <c r="F33" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="G33" t="s">
-        <v>39</v>
+        <v>24</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
@@ -1458,10 +1457,10 @@
         <v>22</v>
       </c>
       <c r="C34" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D34" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="E34" t="s">
         <v>13</v>
@@ -1470,7 +1469,7 @@
         <v>20</v>
       </c>
       <c r="G34" t="s">
-        <v>39</v>
+        <v>24</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
@@ -1481,10 +1480,10 @@
         <v>22</v>
       </c>
       <c r="C35" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D35" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="E35" t="s">
         <v>13</v>
@@ -1493,7 +1492,7 @@
         <v>21</v>
       </c>
       <c r="G35" t="s">
-        <v>39</v>
+        <v>24</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
@@ -1504,10 +1503,10 @@
         <v>22</v>
       </c>
       <c r="C36" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D36" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="E36" t="s">
         <v>13</v>
@@ -1516,7 +1515,7 @@
         <v>12</v>
       </c>
       <c r="G36" t="s">
-        <v>39</v>
+        <v>24</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
@@ -1527,10 +1526,10 @@
         <v>23</v>
       </c>
       <c r="C37" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D37" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="E37" t="s">
         <v>12</v>
@@ -1539,7 +1538,7 @@
         <v>20</v>
       </c>
       <c r="G37" t="s">
-        <v>12</v>
+        <v>44</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
@@ -1550,10 +1549,10 @@
         <v>22</v>
       </c>
       <c r="C38" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D38" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="E38" t="s">
         <v>12</v>
@@ -1562,7 +1561,7 @@
         <v>20</v>
       </c>
       <c r="G38" t="s">
-        <v>39</v>
+        <v>24</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
@@ -1573,10 +1572,10 @@
         <v>23</v>
       </c>
       <c r="C39" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D39" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="E39" t="s">
         <v>12</v>
@@ -1585,7 +1584,7 @@
         <v>20</v>
       </c>
       <c r="G39" t="s">
-        <v>12</v>
+        <v>44</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
@@ -1596,10 +1595,10 @@
         <v>23</v>
       </c>
       <c r="C40" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D40" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="E40" t="s">
         <v>12</v>
@@ -1608,7 +1607,7 @@
         <v>20</v>
       </c>
       <c r="G40" t="s">
-        <v>12</v>
+        <v>44</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
@@ -1619,10 +1618,10 @@
         <v>22</v>
       </c>
       <c r="C41" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D41" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="E41" t="s">
         <v>12</v>
@@ -1631,7 +1630,7 @@
         <v>20</v>
       </c>
       <c r="G41" t="s">
-        <v>12</v>
+        <v>44</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
@@ -1642,10 +1641,10 @@
         <v>23</v>
       </c>
       <c r="C42" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D42" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="E42" t="s">
         <v>12</v>
@@ -1654,7 +1653,7 @@
         <v>20</v>
       </c>
       <c r="G42" t="s">
-        <v>12</v>
+        <v>44</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
@@ -1665,10 +1664,10 @@
         <v>23</v>
       </c>
       <c r="C43" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D43" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="E43" t="s">
         <v>12</v>
@@ -1677,7 +1676,7 @@
         <v>12</v>
       </c>
       <c r="G43" t="s">
-        <v>12</v>
+        <v>44</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
@@ -1688,10 +1687,10 @@
         <v>22</v>
       </c>
       <c r="C44" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D44" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="E44" t="s">
         <v>12</v>
@@ -1700,7 +1699,7 @@
         <v>12</v>
       </c>
       <c r="G44" t="s">
-        <v>12</v>
+        <v>45</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
@@ -1711,10 +1710,10 @@
         <v>23</v>
       </c>
       <c r="C45" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D45" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="E45" t="s">
         <v>12</v>
@@ -1723,10 +1722,10 @@
         <v>12</v>
       </c>
       <c r="G45" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>23</v>
       </c>
@@ -1734,45 +1733,45 @@
         <v>22</v>
       </c>
       <c r="C46" t="s">
+        <v>31</v>
+      </c>
+      <c r="D46" t="s">
+        <v>30</v>
+      </c>
+      <c r="E46" t="s">
         <v>28</v>
       </c>
-      <c r="D46" t="s">
-        <v>27</v>
-      </c>
-      <c r="E46" t="s">
+      <c r="F46" t="s">
+        <v>30</v>
+      </c>
+      <c r="G46" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>22</v>
+      </c>
+      <c r="B47" t="s">
+        <v>23</v>
+      </c>
+      <c r="C47" t="s">
+        <v>31</v>
+      </c>
+      <c r="D47" t="s">
+        <v>30</v>
+      </c>
+      <c r="E47" t="s">
+        <v>28</v>
+      </c>
+      <c r="F47" t="s">
+        <v>30</v>
+      </c>
+      <c r="G47" t="s">
         <v>25</v>
       </c>
-      <c r="F46" t="s">
-        <v>27</v>
-      </c>
-      <c r="G46" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>22</v>
-      </c>
-      <c r="B47" t="s">
-        <v>23</v>
-      </c>
-      <c r="C47" t="s">
-        <v>28</v>
-      </c>
-      <c r="D47" t="s">
-        <v>27</v>
-      </c>
-      <c r="E47" t="s">
-        <v>25</v>
-      </c>
-      <c r="F47" t="s">
-        <v>27</v>
-      </c>
-      <c r="G47" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>23</v>
       </c>
@@ -1780,22 +1779,22 @@
         <v>22</v>
       </c>
       <c r="C48" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="D48" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="E48" t="s">
         <v>19</v>
       </c>
       <c r="F48" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="G48" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>22</v>
       </c>
@@ -1803,22 +1802,22 @@
         <v>23</v>
       </c>
       <c r="C49" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="D49" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="E49" t="s">
         <v>19</v>
       </c>
       <c r="F49" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="G49" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>23</v>
       </c>
@@ -1826,22 +1825,22 @@
         <v>22</v>
       </c>
       <c r="C50" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="D50" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="E50" t="s">
         <v>13</v>
       </c>
       <c r="F50" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="G50" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>22</v>
       </c>
@@ -1849,22 +1848,22 @@
         <v>23</v>
       </c>
       <c r="C51" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="D51" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="E51" t="s">
         <v>13</v>
       </c>
       <c r="F51" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="G51" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>23</v>
       </c>
@@ -1872,91 +1871,91 @@
         <v>22</v>
       </c>
       <c r="C52" t="s">
+        <v>31</v>
+      </c>
+      <c r="D52" t="s">
+        <v>30</v>
+      </c>
+      <c r="E52" t="s">
+        <v>12</v>
+      </c>
+      <c r="F52" t="s">
+        <v>30</v>
+      </c>
+      <c r="G52" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>23</v>
+      </c>
+      <c r="B53" t="s">
+        <v>22</v>
+      </c>
+      <c r="C53" t="s">
+        <v>31</v>
+      </c>
+      <c r="D53" t="s">
+        <v>30</v>
+      </c>
+      <c r="E53" t="s">
+        <v>12</v>
+      </c>
+      <c r="F53" t="s">
+        <v>30</v>
+      </c>
+      <c r="G53" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>22</v>
+      </c>
+      <c r="B54" t="s">
+        <v>23</v>
+      </c>
+      <c r="C54" t="s">
+        <v>31</v>
+      </c>
+      <c r="D54" t="s">
+        <v>30</v>
+      </c>
+      <c r="E54" t="s">
+        <v>12</v>
+      </c>
+      <c r="F54" t="s">
+        <v>30</v>
+      </c>
+      <c r="G54" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>23</v>
+      </c>
+      <c r="B55" t="s">
+        <v>23</v>
+      </c>
+      <c r="C55" t="s">
+        <v>31</v>
+      </c>
+      <c r="D55" t="s">
+        <v>41</v>
+      </c>
+      <c r="E55" t="s">
         <v>28</v>
       </c>
-      <c r="D52" t="s">
-        <v>27</v>
-      </c>
-      <c r="E52" t="s">
-        <v>12</v>
-      </c>
-      <c r="F52" t="s">
-        <v>27</v>
-      </c>
-      <c r="G52" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>23</v>
-      </c>
-      <c r="B53" t="s">
-        <v>22</v>
-      </c>
-      <c r="C53" t="s">
-        <v>28</v>
-      </c>
-      <c r="D53" t="s">
-        <v>27</v>
-      </c>
-      <c r="E53" t="s">
-        <v>12</v>
-      </c>
-      <c r="F53" t="s">
-        <v>27</v>
-      </c>
-      <c r="G53" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>22</v>
-      </c>
-      <c r="B54" t="s">
-        <v>23</v>
-      </c>
-      <c r="C54" t="s">
-        <v>28</v>
-      </c>
-      <c r="D54" t="s">
-        <v>27</v>
-      </c>
-      <c r="E54" t="s">
-        <v>12</v>
-      </c>
-      <c r="F54" t="s">
-        <v>27</v>
-      </c>
-      <c r="G54" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>23</v>
-      </c>
-      <c r="B55" t="s">
-        <v>23</v>
-      </c>
-      <c r="C55" t="s">
-        <v>28</v>
-      </c>
-      <c r="D55" t="s">
-        <v>44</v>
-      </c>
-      <c r="E55" t="s">
-        <v>25</v>
-      </c>
       <c r="F55" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="G55" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>23</v>
       </c>
@@ -1964,22 +1963,22 @@
         <v>23</v>
       </c>
       <c r="C56" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="D56" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E56" t="s">
         <v>19</v>
       </c>
       <c r="F56" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="G56" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>23</v>
       </c>
@@ -1987,22 +1986,22 @@
         <v>23</v>
       </c>
       <c r="C57" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="D57" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E57" t="s">
         <v>13</v>
       </c>
       <c r="F57" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="G57" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>23</v>
       </c>
@@ -2010,68 +2009,68 @@
         <v>23</v>
       </c>
       <c r="C58" t="s">
+        <v>31</v>
+      </c>
+      <c r="D58" t="s">
+        <v>41</v>
+      </c>
+      <c r="E58" t="s">
+        <v>12</v>
+      </c>
+      <c r="F58" t="s">
+        <v>30</v>
+      </c>
+      <c r="G58" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>23</v>
+      </c>
+      <c r="B59" t="s">
+        <v>23</v>
+      </c>
+      <c r="C59" t="s">
+        <v>31</v>
+      </c>
+      <c r="D59" t="s">
+        <v>40</v>
+      </c>
+      <c r="E59" t="s">
         <v>28</v>
       </c>
-      <c r="D58" t="s">
-        <v>44</v>
-      </c>
-      <c r="E58" t="s">
-        <v>12</v>
-      </c>
-      <c r="F58" t="s">
-        <v>27</v>
-      </c>
-      <c r="G58" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>23</v>
-      </c>
-      <c r="B59" t="s">
-        <v>23</v>
-      </c>
-      <c r="C59" t="s">
-        <v>28</v>
-      </c>
-      <c r="D59" t="s">
-        <v>43</v>
-      </c>
-      <c r="E59" t="s">
+      <c r="F59" t="s">
+        <v>30</v>
+      </c>
+      <c r="G59" t="s">
         <v>25</v>
       </c>
-      <c r="F59" t="s">
-        <v>27</v>
-      </c>
-      <c r="G59" t="s">
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>23</v>
+      </c>
+      <c r="B60" t="s">
+        <v>23</v>
+      </c>
+      <c r="C60" t="s">
+        <v>31</v>
+      </c>
+      <c r="D60" t="s">
         <v>40</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
-        <v>23</v>
-      </c>
-      <c r="B60" t="s">
-        <v>23</v>
-      </c>
-      <c r="C60" t="s">
-        <v>28</v>
-      </c>
-      <c r="D60" t="s">
-        <v>43</v>
       </c>
       <c r="E60" t="s">
         <v>19</v>
       </c>
       <c r="F60" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="G60" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>23</v>
       </c>
@@ -2079,22 +2078,22 @@
         <v>23</v>
       </c>
       <c r="C61" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="D61" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E61" t="s">
         <v>13</v>
       </c>
       <c r="F61" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="G61" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="62" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>23</v>
       </c>
@@ -2102,22 +2101,22 @@
         <v>23</v>
       </c>
       <c r="C62" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="D62" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E62" t="s">
         <v>12</v>
       </c>
       <c r="F62" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="G62" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="63" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>23</v>
       </c>
@@ -2125,22 +2124,22 @@
         <v>23</v>
       </c>
       <c r="C63" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="D63" t="s">
         <v>14</v>
       </c>
       <c r="E63" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="F63" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="G63" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="64" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>23</v>
       </c>
@@ -2148,7 +2147,7 @@
         <v>23</v>
       </c>
       <c r="C64" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="D64" t="s">
         <v>14</v>
@@ -2157,13 +2156,13 @@
         <v>19</v>
       </c>
       <c r="F64" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="G64" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="65" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>23</v>
       </c>
@@ -2171,7 +2170,7 @@
         <v>23</v>
       </c>
       <c r="C65" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="D65" t="s">
         <v>14</v>
@@ -2180,13 +2179,13 @@
         <v>13</v>
       </c>
       <c r="F65" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="G65" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="66" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>23</v>
       </c>
@@ -2194,7 +2193,7 @@
         <v>23</v>
       </c>
       <c r="C66" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="D66" t="s">
         <v>14</v>
@@ -2203,13 +2202,13 @@
         <v>12</v>
       </c>
       <c r="F66" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="G66" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="67" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>23</v>
       </c>
@@ -2217,22 +2216,22 @@
         <v>23</v>
       </c>
       <c r="C67" t="s">
+        <v>31</v>
+      </c>
+      <c r="D67" t="s">
+        <v>12</v>
+      </c>
+      <c r="E67" t="s">
         <v>28</v>
       </c>
-      <c r="D67" t="s">
-        <v>12</v>
-      </c>
-      <c r="E67" t="s">
-        <v>25</v>
-      </c>
       <c r="F67" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="G67" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="68" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>23</v>
       </c>
@@ -2240,7 +2239,7 @@
         <v>23</v>
       </c>
       <c r="C68" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="D68" t="s">
         <v>12</v>
@@ -2249,13 +2248,13 @@
         <v>19</v>
       </c>
       <c r="F68" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="G68" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="69" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>23</v>
       </c>
@@ -2263,7 +2262,7 @@
         <v>23</v>
       </c>
       <c r="C69" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="D69" t="s">
         <v>12</v>
@@ -2272,13 +2271,13 @@
         <v>13</v>
       </c>
       <c r="F69" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="G69" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="70" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>23</v>
       </c>
@@ -2286,91 +2285,91 @@
         <v>23</v>
       </c>
       <c r="C70" t="s">
+        <v>31</v>
+      </c>
+      <c r="D70" t="s">
+        <v>12</v>
+      </c>
+      <c r="E70" t="s">
+        <v>12</v>
+      </c>
+      <c r="F70" t="s">
+        <v>30</v>
+      </c>
+      <c r="G70" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>23</v>
+      </c>
+      <c r="B71" t="s">
+        <v>23</v>
+      </c>
+      <c r="C71" t="s">
+        <v>32</v>
+      </c>
+      <c r="D71" t="s">
+        <v>30</v>
+      </c>
+      <c r="E71" t="s">
+        <v>30</v>
+      </c>
+      <c r="F71" t="s">
+        <v>30</v>
+      </c>
+      <c r="G71" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>22</v>
+      </c>
+      <c r="B72" t="s">
+        <v>23</v>
+      </c>
+      <c r="C72" t="s">
+        <v>32</v>
+      </c>
+      <c r="D72" t="s">
+        <v>30</v>
+      </c>
+      <c r="E72" t="s">
+        <v>30</v>
+      </c>
+      <c r="F72" t="s">
+        <v>30</v>
+      </c>
+      <c r="G72" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>23</v>
+      </c>
+      <c r="B73" t="s">
+        <v>22</v>
+      </c>
+      <c r="C73" t="s">
+        <v>32</v>
+      </c>
+      <c r="D73" t="s">
+        <v>30</v>
+      </c>
+      <c r="E73" t="s">
         <v>28</v>
       </c>
-      <c r="D70" t="s">
-        <v>12</v>
-      </c>
-      <c r="E70" t="s">
-        <v>12</v>
-      </c>
-      <c r="F70" t="s">
-        <v>27</v>
-      </c>
-      <c r="G70" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="71" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
-        <v>23</v>
-      </c>
-      <c r="B71" t="s">
-        <v>23</v>
-      </c>
-      <c r="C71" t="s">
-        <v>29</v>
-      </c>
-      <c r="D71" t="s">
-        <v>27</v>
-      </c>
-      <c r="E71" t="s">
-        <v>27</v>
-      </c>
-      <c r="F71" t="s">
-        <v>27</v>
-      </c>
-      <c r="G71" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="72" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
-        <v>22</v>
-      </c>
-      <c r="B72" t="s">
-        <v>23</v>
-      </c>
-      <c r="C72" t="s">
-        <v>29</v>
-      </c>
-      <c r="D72" t="s">
-        <v>27</v>
-      </c>
-      <c r="E72" t="s">
-        <v>27</v>
-      </c>
-      <c r="F72" t="s">
-        <v>27</v>
-      </c>
-      <c r="G72" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="73" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
-        <v>23</v>
-      </c>
-      <c r="B73" t="s">
-        <v>22</v>
-      </c>
-      <c r="C73" t="s">
-        <v>29</v>
-      </c>
-      <c r="D73" t="s">
-        <v>27</v>
-      </c>
-      <c r="E73" t="s">
-        <v>25</v>
-      </c>
       <c r="F73" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="G73" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="74" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>23</v>
       </c>
@@ -2378,22 +2377,22 @@
         <v>22</v>
       </c>
       <c r="C74" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="D74" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="E74" t="s">
         <v>19</v>
       </c>
       <c r="F74" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="G74" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="75" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>23</v>
       </c>
@@ -2401,22 +2400,22 @@
         <v>22</v>
       </c>
       <c r="C75" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="D75" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="E75" t="s">
         <v>13</v>
       </c>
       <c r="F75" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="G75" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="76" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>23</v>
       </c>
@@ -2424,22 +2423,22 @@
         <v>22</v>
       </c>
       <c r="C76" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="D76" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="E76" t="s">
         <v>12</v>
       </c>
       <c r="F76" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="G76" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="77" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>23</v>
       </c>
@@ -2450,19 +2449,19 @@
         <v>12</v>
       </c>
       <c r="D77" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="E77" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="F77" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="G77" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="78" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>22</v>
       </c>
@@ -2473,19 +2472,19 @@
         <v>12</v>
       </c>
       <c r="D78" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="E78" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="F78" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="G78" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="79" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>23</v>
       </c>
@@ -2496,19 +2495,19 @@
         <v>12</v>
       </c>
       <c r="D79" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="E79" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="F79" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="G79" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="80" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>23</v>
       </c>
@@ -2519,19 +2518,19 @@
         <v>12</v>
       </c>
       <c r="D80" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="E80" t="s">
         <v>19</v>
       </c>
       <c r="F80" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="G80" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="81" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>23</v>
       </c>
@@ -2542,19 +2541,19 @@
         <v>12</v>
       </c>
       <c r="D81" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="E81" t="s">
         <v>13</v>
       </c>
       <c r="F81" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="G81" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="82" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>23</v>
       </c>
@@ -2565,26 +2564,20 @@
         <v>12</v>
       </c>
       <c r="D82" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="E82" t="s">
         <v>12</v>
       </c>
       <c r="F82" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="G82" t="s">
-        <v>12</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G82" xr:uid="{920955FF-C75C-492B-A53F-AFC4A746FDCE}">
-    <filterColumn colId="2">
-      <filters>
-        <filter val="(-3.0 .. -1.6]"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:G82" xr:uid="{920955FF-C75C-492B-A53F-AFC4A746FDCE}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G65">
     <sortCondition ref="E2:E65"/>
     <sortCondition ref="C2:C65"/>
@@ -2630,10 +2623,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -2679,7 +2672,7 @@
         <v>12</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>12</v>
@@ -2693,7 +2686,7 @@
         <v>5</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>23</v>
@@ -2746,10 +2739,10 @@
         <v>10</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>22</v>
@@ -2805,7 +2798,7 @@
         <v>5</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="D11" s="5" t="s">
         <v>23</v>
@@ -2869,7 +2862,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2882,10 +2875,10 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>37</v>
@@ -2893,7 +2886,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>6</v>
@@ -2904,10 +2897,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C3" s="7" t="s">
         <v>23</v>
@@ -2915,7 +2908,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>7</v>
@@ -2926,7 +2919,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>36</v>

</xml_diff>

<commit_message>
Aanpassingen pre- en postbewerkingen
</commit_message>
<xml_diff>
--- a/src/main/resources/nhs-dmn/CHgestript.xlsx
+++ b/src/main/resources/nhs-dmn/CHgestript.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-20.04\home\han\git\rivm\nhs\dmn\nhs-business\src\main\resources\nhs-dmn\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{270E6B09-B1AC-4C35-AB73-29D9E107077C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69E0DE1C-5D2A-4990-AFC3-ADF80714DFF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="834" xr2:uid="{4203C9A5-FA6C-4E14-8325-EE7186AD0D41}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="834" activeTab="3" xr2:uid="{4203C9A5-FA6C-4E14-8325-EE7186AD0D41}"/>
   </bookViews>
   <sheets>
     <sheet name="MeetResultaat" sheetId="22" r:id="rId1"/>
@@ -52,19 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="647" uniqueCount="46">
-  <si>
-    <t>T4</t>
-  </si>
-  <si>
-    <t>TSH</t>
-  </si>
-  <si>
-    <t>TBG</t>
-  </si>
-  <si>
-    <t>T4/TBG</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="647" uniqueCount="48">
   <si>
     <t>&lt;= 252</t>
   </si>
@@ -180,16 +168,34 @@
     <t>(40 .. 105]</t>
   </si>
   <si>
-    <t>hielprik.hielprikType</t>
-  </si>
-  <si>
-    <t>onbekend(hielprik,"T4")</t>
-  </si>
-  <si>
-    <t>onbekend(hielprik,"TSH")</t>
-  </si>
-  <si>
-    <t>onbekend(hielprik,"T4/TBG")</t>
+    <t>nhsCommon.onbekend(nhsCommon.hielprik,"TSH")</t>
+  </si>
+  <si>
+    <t>nhsCommon.onbekend(nhsCommon.hielprik,"T4")</t>
+  </si>
+  <si>
+    <t>nhsCommon.onbekend(nhsCommon.hielprik,"T4/TBG")</t>
+  </si>
+  <si>
+    <t>nhsCommon.isPrematuur</t>
+  </si>
+  <si>
+    <t>nhsCommon.THP</t>
+  </si>
+  <si>
+    <t>nhsCommon.T4</t>
+  </si>
+  <si>
+    <t>nhsCommon.TBG</t>
+  </si>
+  <si>
+    <t>nhsCommon.TSH</t>
+  </si>
+  <si>
+    <t>nhsCommon."T4/TBG"</t>
+  </si>
+  <si>
+    <t>nhsCommon.hielprik.hielprikType</t>
   </si>
 </sst>
 </file>
@@ -675,7 +681,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{920955FF-C75C-492B-A53F-AFC4A746FDCE}">
   <dimension ref="A1:G82"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="H1" sqref="H1:H1048576"/>
     </sheetView>
@@ -687,1893 +693,1893 @@
     <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="48.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>15</v>
+        <v>41</v>
       </c>
       <c r="B1" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="C1" t="s">
-        <v>0</v>
+        <v>43</v>
       </c>
       <c r="D1" t="s">
-        <v>2</v>
+        <v>44</v>
       </c>
       <c r="E1" t="s">
-        <v>1</v>
+        <v>45</v>
       </c>
       <c r="F1" t="s">
-        <v>3</v>
+        <v>46</v>
       </c>
       <c r="G1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B2" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C2" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D2" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E2" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="F2" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="G2" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" t="s">
+        <v>26</v>
+      </c>
+      <c r="G3" t="s">
         <v>22</v>
-      </c>
-      <c r="B3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D3" t="s">
-        <v>30</v>
-      </c>
-      <c r="E3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F3" t="s">
-        <v>30</v>
-      </c>
-      <c r="G3" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B4" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C4" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D4" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E4" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F4" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="G4" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B5" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C5" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D5" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E5" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F5" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="G5" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B6" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C6" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D6" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E6" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="F6" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="G6" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B7" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C7" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D7" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E7" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="F7" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="G7" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B8" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C8" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D8" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E8" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="F8" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="G8" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B9" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C9" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D9" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E9" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="F9" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="G9" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" t="s">
+        <v>26</v>
+      </c>
+      <c r="E10" t="s">
+        <v>15</v>
+      </c>
+      <c r="F10" t="s">
+        <v>26</v>
+      </c>
+      <c r="G10" t="s">
         <v>22</v>
-      </c>
-      <c r="C10" t="s">
-        <v>29</v>
-      </c>
-      <c r="D10" t="s">
-        <v>30</v>
-      </c>
-      <c r="E10" t="s">
-        <v>19</v>
-      </c>
-      <c r="F10" t="s">
-        <v>30</v>
-      </c>
-      <c r="G10" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" t="s">
+        <v>26</v>
+      </c>
+      <c r="E11" t="s">
+        <v>15</v>
+      </c>
+      <c r="F11" t="s">
+        <v>26</v>
+      </c>
+      <c r="G11" t="s">
         <v>22</v>
-      </c>
-      <c r="B11" t="s">
-        <v>23</v>
-      </c>
-      <c r="C11" t="s">
-        <v>29</v>
-      </c>
-      <c r="D11" t="s">
-        <v>30</v>
-      </c>
-      <c r="E11" t="s">
-        <v>19</v>
-      </c>
-      <c r="F11" t="s">
-        <v>30</v>
-      </c>
-      <c r="G11" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B12" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C12" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D12" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E12" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F12" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="G12" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B13" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C13" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D13" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E13" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F13" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="G13" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B14" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C14" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D14" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E14" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F14" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="G14" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B15" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C15" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D15" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E15" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F15" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="G15" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B16" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C16" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D16" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E16" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F16" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="G16" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B17" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C17" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D17" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E17" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F17" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="G17" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18" t="s">
         <v>23</v>
       </c>
-      <c r="B18" t="s">
-        <v>23</v>
-      </c>
-      <c r="C18" t="s">
-        <v>27</v>
-      </c>
       <c r="D18" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E18" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="F18" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="G18" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B19" t="s">
+        <v>19</v>
+      </c>
+      <c r="C19" t="s">
         <v>23</v>
       </c>
-      <c r="C19" t="s">
-        <v>27</v>
-      </c>
       <c r="D19" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E19" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="F19" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="G19" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>18</v>
+      </c>
+      <c r="C20" t="s">
         <v>23</v>
       </c>
-      <c r="B20" t="s">
-        <v>22</v>
-      </c>
-      <c r="C20" t="s">
-        <v>27</v>
-      </c>
       <c r="D20" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E20" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="F20" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="G20" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>19</v>
+      </c>
+      <c r="B21" t="s">
+        <v>18</v>
+      </c>
+      <c r="C21" t="s">
         <v>23</v>
       </c>
-      <c r="B21" t="s">
-        <v>22</v>
-      </c>
-      <c r="C21" t="s">
-        <v>27</v>
-      </c>
       <c r="D21" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E21" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="F21" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="G21" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>19</v>
+      </c>
+      <c r="B22" t="s">
+        <v>18</v>
+      </c>
+      <c r="C22" t="s">
         <v>23</v>
       </c>
-      <c r="B22" t="s">
-        <v>22</v>
-      </c>
-      <c r="C22" t="s">
-        <v>27</v>
-      </c>
       <c r="D22" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E22" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="F22" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="G22" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>19</v>
+      </c>
+      <c r="B23" t="s">
+        <v>19</v>
+      </c>
+      <c r="C23" t="s">
         <v>23</v>
       </c>
-      <c r="B23" t="s">
-        <v>23</v>
-      </c>
-      <c r="C23" t="s">
-        <v>27</v>
-      </c>
       <c r="D23" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E23" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="F23" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="G23" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>19</v>
+      </c>
+      <c r="B24" t="s">
+        <v>18</v>
+      </c>
+      <c r="C24" t="s">
         <v>23</v>
       </c>
-      <c r="B24" t="s">
-        <v>22</v>
-      </c>
-      <c r="C24" t="s">
-        <v>27</v>
-      </c>
       <c r="D24" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E24" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="F24" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="G24" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>18</v>
+      </c>
+      <c r="B25" t="s">
+        <v>19</v>
+      </c>
+      <c r="C25" t="s">
+        <v>23</v>
+      </c>
+      <c r="D25" t="s">
+        <v>26</v>
+      </c>
+      <c r="E25" t="s">
+        <v>15</v>
+      </c>
+      <c r="F25" t="s">
+        <v>16</v>
+      </c>
+      <c r="G25" t="s">
         <v>22</v>
-      </c>
-      <c r="B25" t="s">
-        <v>23</v>
-      </c>
-      <c r="C25" t="s">
-        <v>27</v>
-      </c>
-      <c r="D25" t="s">
-        <v>30</v>
-      </c>
-      <c r="E25" t="s">
-        <v>19</v>
-      </c>
-      <c r="F25" t="s">
-        <v>20</v>
-      </c>
-      <c r="G25" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
+        <v>19</v>
+      </c>
+      <c r="B26" t="s">
+        <v>19</v>
+      </c>
+      <c r="C26" t="s">
         <v>23</v>
       </c>
-      <c r="B26" t="s">
-        <v>23</v>
-      </c>
-      <c r="C26" t="s">
-        <v>27</v>
-      </c>
       <c r="D26" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E26" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="F26" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="G26" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
+        <v>19</v>
+      </c>
+      <c r="B27" t="s">
+        <v>18</v>
+      </c>
+      <c r="C27" t="s">
         <v>23</v>
       </c>
-      <c r="B27" t="s">
+      <c r="D27" t="s">
+        <v>26</v>
+      </c>
+      <c r="E27" t="s">
+        <v>15</v>
+      </c>
+      <c r="F27" t="s">
+        <v>17</v>
+      </c>
+      <c r="G27" t="s">
         <v>22</v>
-      </c>
-      <c r="C27" t="s">
-        <v>27</v>
-      </c>
-      <c r="D27" t="s">
-        <v>30</v>
-      </c>
-      <c r="E27" t="s">
-        <v>19</v>
-      </c>
-      <c r="F27" t="s">
-        <v>21</v>
-      </c>
-      <c r="G27" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
+        <v>18</v>
+      </c>
+      <c r="B28" t="s">
+        <v>19</v>
+      </c>
+      <c r="C28" t="s">
+        <v>23</v>
+      </c>
+      <c r="D28" t="s">
+        <v>26</v>
+      </c>
+      <c r="E28" t="s">
+        <v>15</v>
+      </c>
+      <c r="F28" t="s">
+        <v>17</v>
+      </c>
+      <c r="G28" t="s">
         <v>22</v>
-      </c>
-      <c r="B28" t="s">
-        <v>23</v>
-      </c>
-      <c r="C28" t="s">
-        <v>27</v>
-      </c>
-      <c r="D28" t="s">
-        <v>30</v>
-      </c>
-      <c r="E28" t="s">
-        <v>19</v>
-      </c>
-      <c r="F28" t="s">
-        <v>21</v>
-      </c>
-      <c r="G28" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
+        <v>19</v>
+      </c>
+      <c r="B29" t="s">
+        <v>19</v>
+      </c>
+      <c r="C29" t="s">
         <v>23</v>
       </c>
-      <c r="B29" t="s">
-        <v>23</v>
-      </c>
-      <c r="C29" t="s">
-        <v>27</v>
-      </c>
       <c r="D29" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E29" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="F29" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="G29" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
+        <v>19</v>
+      </c>
+      <c r="B30" t="s">
+        <v>18</v>
+      </c>
+      <c r="C30" t="s">
         <v>23</v>
       </c>
-      <c r="B30" t="s">
-        <v>22</v>
-      </c>
-      <c r="C30" t="s">
-        <v>27</v>
-      </c>
       <c r="D30" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E30" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="F30" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="G30" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
+        <v>18</v>
+      </c>
+      <c r="B31" t="s">
+        <v>19</v>
+      </c>
+      <c r="C31" t="s">
+        <v>23</v>
+      </c>
+      <c r="D31" t="s">
+        <v>26</v>
+      </c>
+      <c r="E31" t="s">
+        <v>15</v>
+      </c>
+      <c r="F31" t="s">
+        <v>8</v>
+      </c>
+      <c r="G31" t="s">
         <v>22</v>
-      </c>
-      <c r="B31" t="s">
-        <v>23</v>
-      </c>
-      <c r="C31" t="s">
-        <v>27</v>
-      </c>
-      <c r="D31" t="s">
-        <v>30</v>
-      </c>
-      <c r="E31" t="s">
-        <v>19</v>
-      </c>
-      <c r="F31" t="s">
-        <v>12</v>
-      </c>
-      <c r="G31" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
+        <v>19</v>
+      </c>
+      <c r="B32" t="s">
+        <v>19</v>
+      </c>
+      <c r="C32" t="s">
         <v>23</v>
       </c>
-      <c r="B32" t="s">
-        <v>23</v>
-      </c>
-      <c r="C32" t="s">
-        <v>27</v>
-      </c>
       <c r="D32" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E32" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F32" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="G32" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B33" t="s">
+        <v>19</v>
+      </c>
+      <c r="C33" t="s">
         <v>23</v>
       </c>
-      <c r="C33" t="s">
-        <v>27</v>
-      </c>
       <c r="D33" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E33" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F33" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="G33" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
+        <v>19</v>
+      </c>
+      <c r="B34" t="s">
+        <v>18</v>
+      </c>
+      <c r="C34" t="s">
         <v>23</v>
       </c>
-      <c r="B34" t="s">
-        <v>22</v>
-      </c>
-      <c r="C34" t="s">
-        <v>27</v>
-      </c>
       <c r="D34" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E34" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F34" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="G34" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
+        <v>19</v>
+      </c>
+      <c r="B35" t="s">
+        <v>18</v>
+      </c>
+      <c r="C35" t="s">
         <v>23</v>
       </c>
-      <c r="B35" t="s">
-        <v>22</v>
-      </c>
-      <c r="C35" t="s">
-        <v>27</v>
-      </c>
       <c r="D35" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E35" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F35" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="G35" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
+        <v>19</v>
+      </c>
+      <c r="B36" t="s">
+        <v>18</v>
+      </c>
+      <c r="C36" t="s">
         <v>23</v>
       </c>
-      <c r="B36" t="s">
-        <v>22</v>
-      </c>
-      <c r="C36" t="s">
-        <v>27</v>
-      </c>
       <c r="D36" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E36" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F36" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="G36" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
+        <v>19</v>
+      </c>
+      <c r="B37" t="s">
+        <v>19</v>
+      </c>
+      <c r="C37" t="s">
         <v>23</v>
       </c>
-      <c r="B37" t="s">
-        <v>23</v>
-      </c>
-      <c r="C37" t="s">
-        <v>27</v>
-      </c>
       <c r="D37" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E37" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F37" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="G37" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
+        <v>19</v>
+      </c>
+      <c r="B38" t="s">
+        <v>18</v>
+      </c>
+      <c r="C38" t="s">
         <v>23</v>
       </c>
-      <c r="B38" t="s">
-        <v>22</v>
-      </c>
-      <c r="C38" t="s">
-        <v>27</v>
-      </c>
       <c r="D38" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E38" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F38" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="G38" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B39" t="s">
+        <v>19</v>
+      </c>
+      <c r="C39" t="s">
         <v>23</v>
       </c>
-      <c r="C39" t="s">
-        <v>27</v>
-      </c>
       <c r="D39" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E39" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F39" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="G39" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
+        <v>19</v>
+      </c>
+      <c r="B40" t="s">
+        <v>19</v>
+      </c>
+      <c r="C40" t="s">
         <v>23</v>
       </c>
-      <c r="B40" t="s">
-        <v>23</v>
-      </c>
-      <c r="C40" t="s">
-        <v>27</v>
-      </c>
       <c r="D40" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E40" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F40" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="G40" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
+        <v>19</v>
+      </c>
+      <c r="B41" t="s">
+        <v>18</v>
+      </c>
+      <c r="C41" t="s">
         <v>23</v>
       </c>
-      <c r="B41" t="s">
-        <v>22</v>
-      </c>
-      <c r="C41" t="s">
-        <v>27</v>
-      </c>
       <c r="D41" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E41" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F41" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="G41" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B42" t="s">
+        <v>19</v>
+      </c>
+      <c r="C42" t="s">
         <v>23</v>
       </c>
-      <c r="C42" t="s">
-        <v>27</v>
-      </c>
       <c r="D42" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E42" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F42" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="G42" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
+        <v>19</v>
+      </c>
+      <c r="B43" t="s">
+        <v>19</v>
+      </c>
+      <c r="C43" t="s">
         <v>23</v>
       </c>
-      <c r="B43" t="s">
-        <v>23</v>
-      </c>
-      <c r="C43" t="s">
-        <v>27</v>
-      </c>
       <c r="D43" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E43" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F43" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="G43" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
+        <v>19</v>
+      </c>
+      <c r="B44" t="s">
+        <v>18</v>
+      </c>
+      <c r="C44" t="s">
         <v>23</v>
       </c>
-      <c r="B44" t="s">
-        <v>22</v>
-      </c>
-      <c r="C44" t="s">
-        <v>27</v>
-      </c>
       <c r="D44" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E44" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F44" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="G44" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B45" t="s">
+        <v>19</v>
+      </c>
+      <c r="C45" t="s">
         <v>23</v>
       </c>
-      <c r="C45" t="s">
-        <v>27</v>
-      </c>
       <c r="D45" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E45" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F45" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="G45" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B46" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C46" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D46" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E46" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="F46" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="G46" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B47" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C47" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D47" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E47" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="F47" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="G47" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B48" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C48" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D48" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E48" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="F48" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="G48" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
+        <v>18</v>
+      </c>
+      <c r="B49" t="s">
+        <v>19</v>
+      </c>
+      <c r="C49" t="s">
+        <v>27</v>
+      </c>
+      <c r="D49" t="s">
+        <v>26</v>
+      </c>
+      <c r="E49" t="s">
+        <v>15</v>
+      </c>
+      <c r="F49" t="s">
+        <v>26</v>
+      </c>
+      <c r="G49" t="s">
         <v>22</v>
-      </c>
-      <c r="B49" t="s">
-        <v>23</v>
-      </c>
-      <c r="C49" t="s">
-        <v>31</v>
-      </c>
-      <c r="D49" t="s">
-        <v>30</v>
-      </c>
-      <c r="E49" t="s">
-        <v>19</v>
-      </c>
-      <c r="F49" t="s">
-        <v>30</v>
-      </c>
-      <c r="G49" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B50" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C50" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D50" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E50" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F50" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="G50" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B51" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C51" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D51" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E51" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F51" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="G51" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B52" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C52" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D52" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E52" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F52" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="G52" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B53" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C53" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D53" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E53" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F53" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="G53" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B54" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C54" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D54" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E54" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F54" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="G54" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B55" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C55" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D55" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="E55" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="F55" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="G55" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B56" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C56" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D56" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="E56" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="F56" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="G56" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B57" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C57" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D57" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="E57" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F57" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="G57" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B58" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C58" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D58" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="E58" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F58" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="G58" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B59" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C59" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D59" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="E59" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="F59" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="G59" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B60" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C60" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D60" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="E60" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="F60" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="G60" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B61" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C61" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D61" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="E61" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F61" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="G61" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B62" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C62" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D62" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="E62" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F62" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="G62" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B63" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C63" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D63" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="E63" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="F63" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="G63" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B64" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C64" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D64" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="E64" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="F64" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="G64" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B65" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C65" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D65" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="E65" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F65" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="G65" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B66" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C66" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D66" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="E66" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F66" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="G66" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B67" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C67" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D67" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E67" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="F67" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="G67" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B68" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C68" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D68" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E68" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="F68" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="G68" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B69" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C69" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D69" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E69" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F69" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="G69" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B70" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C70" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D70" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E70" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F70" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="G70" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B71" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C71" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D71" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E71" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="F71" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="G71" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
+        <v>18</v>
+      </c>
+      <c r="B72" t="s">
+        <v>19</v>
+      </c>
+      <c r="C72" t="s">
+        <v>28</v>
+      </c>
+      <c r="D72" t="s">
+        <v>26</v>
+      </c>
+      <c r="E72" t="s">
+        <v>26</v>
+      </c>
+      <c r="F72" t="s">
+        <v>26</v>
+      </c>
+      <c r="G72" t="s">
         <v>22</v>
-      </c>
-      <c r="B72" t="s">
-        <v>23</v>
-      </c>
-      <c r="C72" t="s">
-        <v>32</v>
-      </c>
-      <c r="D72" t="s">
-        <v>30</v>
-      </c>
-      <c r="E72" t="s">
-        <v>30</v>
-      </c>
-      <c r="F72" t="s">
-        <v>30</v>
-      </c>
-      <c r="G72" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B73" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C73" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D73" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E73" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="F73" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="G73" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B74" t="s">
+        <v>18</v>
+      </c>
+      <c r="C74" t="s">
+        <v>28</v>
+      </c>
+      <c r="D74" t="s">
+        <v>26</v>
+      </c>
+      <c r="E74" t="s">
+        <v>15</v>
+      </c>
+      <c r="F74" t="s">
+        <v>26</v>
+      </c>
+      <c r="G74" t="s">
         <v>22</v>
-      </c>
-      <c r="C74" t="s">
-        <v>32</v>
-      </c>
-      <c r="D74" t="s">
-        <v>30</v>
-      </c>
-      <c r="E74" t="s">
-        <v>19</v>
-      </c>
-      <c r="F74" t="s">
-        <v>30</v>
-      </c>
-      <c r="G74" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B75" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C75" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D75" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E75" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F75" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="G75" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B76" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C76" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D76" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E76" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F76" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="G76" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B77" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C77" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D77" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E77" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="F77" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="G77" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B78" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C78" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D78" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E78" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="F78" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="G78" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B79" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C79" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D79" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E79" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="F79" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="G79" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B80" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C80" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D80" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E80" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="F80" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="G80" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B81" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C81" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D81" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E81" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F81" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="G81" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B82" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C82" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D82" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E82" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F82" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="G82" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -2613,7 +2619,7 @@
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2623,10 +2629,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="B1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -2652,198 +2658,198 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B6" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="4" t="s">
-        <v>8</v>
-      </c>
       <c r="D6" s="5" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B14" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C14" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C14" s="4" t="s">
-        <v>8</v>
-      </c>
       <c r="D14" s="5" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -2861,7 +2867,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCFCADA8-35EC-4674-BB10-19E37C561E05}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
@@ -2875,57 +2881,57 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>33</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
isPrematuur doet het nu
</commit_message>
<xml_diff>
--- a/src/main/resources/nhs-dmn/CHgestript.xlsx
+++ b/src/main/resources/nhs-dmn/CHgestript.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-20.04\home\han\git\rivm\nhs\dmn\nhs-business\src\main\resources\nhs-dmn\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69E0DE1C-5D2A-4990-AFC3-ADF80714DFF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3404C5F6-3EEC-49A7-8603-BBF84A7BF3DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="834" activeTab="3" xr2:uid="{4203C9A5-FA6C-4E14-8325-EE7186AD0D41}"/>
+    <workbookView xWindow="36975" yWindow="4650" windowWidth="28800" windowHeight="11295" tabRatio="834" activeTab="2" xr2:uid="{4203C9A5-FA6C-4E14-8325-EE7186AD0D41}"/>
   </bookViews>
   <sheets>
     <sheet name="MeetResultaat" sheetId="22" r:id="rId1"/>
@@ -90,15 +90,6 @@
     <t>isPrematuur</t>
   </si>
   <si>
-    <t>Zwangerschapsduur</t>
-  </si>
-  <si>
-    <t>AfnametermijnPrematuur</t>
-  </si>
-  <si>
-    <t>Geboortegewicht</t>
-  </si>
-  <si>
     <t>&lt;= 7</t>
   </si>
   <si>
@@ -168,34 +159,43 @@
     <t>(40 .. 105]</t>
   </si>
   <si>
-    <t>nhsCommon.onbekend(nhsCommon.hielprik,"TSH")</t>
-  </si>
-  <si>
-    <t>nhsCommon.onbekend(nhsCommon.hielprik,"T4")</t>
-  </si>
-  <si>
-    <t>nhsCommon.onbekend(nhsCommon.hielprik,"T4/TBG")</t>
-  </si>
-  <si>
-    <t>nhsCommon.isPrematuur</t>
-  </si>
-  <si>
-    <t>nhsCommon.THP</t>
-  </si>
-  <si>
-    <t>nhsCommon.T4</t>
-  </si>
-  <si>
-    <t>nhsCommon.TBG</t>
-  </si>
-  <si>
-    <t>nhsCommon.TSH</t>
-  </si>
-  <si>
-    <t>nhsCommon."T4/TBG"</t>
-  </si>
-  <si>
-    <t>nhsCommon.hielprik.hielprikType</t>
+    <t>hps.isPrematuur</t>
+  </si>
+  <si>
+    <t>hps.THP</t>
+  </si>
+  <si>
+    <t>hps.T4</t>
+  </si>
+  <si>
+    <t>hps.TBG</t>
+  </si>
+  <si>
+    <t>hps.TSH</t>
+  </si>
+  <si>
+    <t>hps."T4/TBG"</t>
+  </si>
+  <si>
+    <t>hps.hielprik.hielprikType</t>
+  </si>
+  <si>
+    <t>hps.redenOnbekend(hps.hielprik,"TSH")</t>
+  </si>
+  <si>
+    <t>hps.redenOnbekend(hps.hielprik,"T4/TBG")</t>
+  </si>
+  <si>
+    <t>hps.redenOnbekend(hps.hielprik,"T4")</t>
+  </si>
+  <si>
+    <t>HPS.AfnametermijnPrematuur</t>
+  </si>
+  <si>
+    <t>HPS.Zwangerschapsduur</t>
+  </si>
+  <si>
+    <t>HPS.Geboortegewicht</t>
   </si>
 </sst>
 </file>
@@ -376,10 +376,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -683,836 +679,837 @@
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H1" sqref="H1:H1048576"/>
+      <selection pane="bottomLeft" sqref="A1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="48.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="40.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="B1" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="C1" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="D1" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="E1" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="F1" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="G1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="F2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C3" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D3" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F3" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C4" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D4" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E4" t="s">
         <v>9</v>
       </c>
       <c r="F4" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G4" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C5" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D5" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E5" t="s">
         <v>8</v>
       </c>
       <c r="F5" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G5" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B6" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C6" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D6" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E6" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="F6" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G6" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B7" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C7" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D7" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E7" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="F7" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G7" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8" t="s">
+        <v>21</v>
+      </c>
+      <c r="F8" t="s">
+        <v>23</v>
+      </c>
+      <c r="G8" t="s">
         <v>18</v>
-      </c>
-      <c r="B8" t="s">
-        <v>19</v>
-      </c>
-      <c r="C8" t="s">
-        <v>25</v>
-      </c>
-      <c r="D8" t="s">
-        <v>26</v>
-      </c>
-      <c r="E8" t="s">
-        <v>24</v>
-      </c>
-      <c r="F8" t="s">
-        <v>26</v>
-      </c>
-      <c r="G8" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" t="s">
+        <v>23</v>
+      </c>
+      <c r="E9" t="s">
+        <v>12</v>
+      </c>
+      <c r="F9" t="s">
+        <v>23</v>
+      </c>
+      <c r="G9" t="s">
         <v>19</v>
-      </c>
-      <c r="B9" t="s">
-        <v>19</v>
-      </c>
-      <c r="C9" t="s">
-        <v>25</v>
-      </c>
-      <c r="D9" t="s">
-        <v>26</v>
-      </c>
-      <c r="E9" t="s">
-        <v>15</v>
-      </c>
-      <c r="F9" t="s">
-        <v>26</v>
-      </c>
-      <c r="G9" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" t="s">
+        <v>23</v>
+      </c>
+      <c r="E10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F10" t="s">
+        <v>23</v>
+      </c>
+      <c r="G10" t="s">
         <v>19</v>
-      </c>
-      <c r="B10" t="s">
-        <v>18</v>
-      </c>
-      <c r="C10" t="s">
-        <v>25</v>
-      </c>
-      <c r="D10" t="s">
-        <v>26</v>
-      </c>
-      <c r="E10" t="s">
-        <v>15</v>
-      </c>
-      <c r="F10" t="s">
-        <v>26</v>
-      </c>
-      <c r="G10" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" t="s">
+        <v>23</v>
+      </c>
+      <c r="E11" t="s">
+        <v>12</v>
+      </c>
+      <c r="F11" t="s">
+        <v>23</v>
+      </c>
+      <c r="G11" t="s">
         <v>19</v>
-      </c>
-      <c r="C11" t="s">
-        <v>25</v>
-      </c>
-      <c r="D11" t="s">
-        <v>26</v>
-      </c>
-      <c r="E11" t="s">
-        <v>15</v>
-      </c>
-      <c r="F11" t="s">
-        <v>26</v>
-      </c>
-      <c r="G11" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B12" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C12" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D12" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E12" t="s">
         <v>9</v>
       </c>
       <c r="F12" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G12" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B13" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C13" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D13" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E13" t="s">
         <v>9</v>
       </c>
       <c r="F13" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G13" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B14" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C14" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D14" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E14" t="s">
         <v>9</v>
       </c>
       <c r="F14" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G14" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B15" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C15" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D15" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E15" t="s">
         <v>8</v>
       </c>
       <c r="F15" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G15" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B16" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C16" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D16" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E16" t="s">
         <v>8</v>
       </c>
       <c r="F16" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G16" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C17" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D17" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E17" t="s">
         <v>8</v>
       </c>
       <c r="F17" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G17" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C18" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D18" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E18" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="F18" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G18" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>15</v>
+      </c>
+      <c r="B19" t="s">
+        <v>16</v>
+      </c>
+      <c r="C19" t="s">
+        <v>20</v>
+      </c>
+      <c r="D19" t="s">
+        <v>23</v>
+      </c>
+      <c r="E19" t="s">
+        <v>21</v>
+      </c>
+      <c r="F19" t="s">
+        <v>23</v>
+      </c>
+      <c r="G19" t="s">
         <v>18</v>
-      </c>
-      <c r="B19" t="s">
-        <v>19</v>
-      </c>
-      <c r="C19" t="s">
-        <v>23</v>
-      </c>
-      <c r="D19" t="s">
-        <v>26</v>
-      </c>
-      <c r="E19" t="s">
-        <v>24</v>
-      </c>
-      <c r="F19" t="s">
-        <v>26</v>
-      </c>
-      <c r="G19" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B20" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C20" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D20" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E20" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="F20" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="G20" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B21" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C21" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D21" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E21" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="F21" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="G21" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B22" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C22" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D22" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E22" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="F22" t="s">
         <v>8</v>
       </c>
       <c r="G22" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B23" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C23" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D23" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E23" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F23" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="G23" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B24" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C24" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D24" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E24" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F24" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="G24" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B25" t="s">
+        <v>16</v>
+      </c>
+      <c r="C25" t="s">
+        <v>20</v>
+      </c>
+      <c r="D25" t="s">
+        <v>23</v>
+      </c>
+      <c r="E25" t="s">
+        <v>12</v>
+      </c>
+      <c r="F25" t="s">
+        <v>13</v>
+      </c>
+      <c r="G25" t="s">
         <v>19</v>
-      </c>
-      <c r="C25" t="s">
-        <v>23</v>
-      </c>
-      <c r="D25" t="s">
-        <v>26</v>
-      </c>
-      <c r="E25" t="s">
-        <v>15</v>
-      </c>
-      <c r="F25" t="s">
-        <v>16</v>
-      </c>
-      <c r="G25" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
+        <v>16</v>
+      </c>
+      <c r="B26" t="s">
+        <v>16</v>
+      </c>
+      <c r="C26" t="s">
+        <v>20</v>
+      </c>
+      <c r="D26" t="s">
+        <v>23</v>
+      </c>
+      <c r="E26" t="s">
+        <v>12</v>
+      </c>
+      <c r="F26" t="s">
+        <v>14</v>
+      </c>
+      <c r="G26" t="s">
         <v>19</v>
-      </c>
-      <c r="B26" t="s">
-        <v>19</v>
-      </c>
-      <c r="C26" t="s">
-        <v>23</v>
-      </c>
-      <c r="D26" t="s">
-        <v>26</v>
-      </c>
-      <c r="E26" t="s">
-        <v>15</v>
-      </c>
-      <c r="F26" t="s">
-        <v>17</v>
-      </c>
-      <c r="G26" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
+        <v>16</v>
+      </c>
+      <c r="B27" t="s">
+        <v>15</v>
+      </c>
+      <c r="C27" t="s">
+        <v>20</v>
+      </c>
+      <c r="D27" t="s">
+        <v>23</v>
+      </c>
+      <c r="E27" t="s">
+        <v>12</v>
+      </c>
+      <c r="F27" t="s">
+        <v>14</v>
+      </c>
+      <c r="G27" t="s">
         <v>19</v>
-      </c>
-      <c r="B27" t="s">
-        <v>18</v>
-      </c>
-      <c r="C27" t="s">
-        <v>23</v>
-      </c>
-      <c r="D27" t="s">
-        <v>26</v>
-      </c>
-      <c r="E27" t="s">
-        <v>15</v>
-      </c>
-      <c r="F27" t="s">
-        <v>17</v>
-      </c>
-      <c r="G27" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B28" t="s">
+        <v>16</v>
+      </c>
+      <c r="C28" t="s">
+        <v>20</v>
+      </c>
+      <c r="D28" t="s">
+        <v>23</v>
+      </c>
+      <c r="E28" t="s">
+        <v>12</v>
+      </c>
+      <c r="F28" t="s">
+        <v>14</v>
+      </c>
+      <c r="G28" t="s">
         <v>19</v>
-      </c>
-      <c r="C28" t="s">
-        <v>23</v>
-      </c>
-      <c r="D28" t="s">
-        <v>26</v>
-      </c>
-      <c r="E28" t="s">
-        <v>15</v>
-      </c>
-      <c r="F28" t="s">
-        <v>17</v>
-      </c>
-      <c r="G28" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B29" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C29" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D29" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E29" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F29" t="s">
         <v>8</v>
       </c>
       <c r="G29" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B30" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C30" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D30" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E30" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F30" t="s">
         <v>8</v>
       </c>
       <c r="G30" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B31" t="s">
+        <v>16</v>
+      </c>
+      <c r="C31" t="s">
+        <v>20</v>
+      </c>
+      <c r="D31" t="s">
+        <v>23</v>
+      </c>
+      <c r="E31" t="s">
+        <v>12</v>
+      </c>
+      <c r="F31" t="s">
+        <v>8</v>
+      </c>
+      <c r="G31" t="s">
         <v>19</v>
-      </c>
-      <c r="C31" t="s">
-        <v>23</v>
-      </c>
-      <c r="D31" t="s">
-        <v>26</v>
-      </c>
-      <c r="E31" t="s">
-        <v>15</v>
-      </c>
-      <c r="F31" t="s">
-        <v>8</v>
-      </c>
-      <c r="G31" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B32" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C32" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D32" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E32" t="s">
         <v>9</v>
       </c>
       <c r="F32" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G32" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B33" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C33" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D33" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E33" t="s">
         <v>9</v>
       </c>
       <c r="F33" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G33" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B34" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C34" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D34" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E34" t="s">
         <v>9</v>
       </c>
       <c r="F34" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="G34" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B35" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C35" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D35" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E35" t="s">
         <v>9</v>
       </c>
       <c r="F35" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="G35" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B36" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C36" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D36" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E36" t="s">
         <v>9</v>
@@ -1521,159 +1518,159 @@
         <v>8</v>
       </c>
       <c r="G36" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B37" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C37" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D37" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E37" t="s">
         <v>8</v>
       </c>
       <c r="F37" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="G37" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B38" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C38" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D38" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E38" t="s">
         <v>8</v>
       </c>
       <c r="F38" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="G38" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B39" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C39" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D39" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E39" t="s">
         <v>8</v>
       </c>
       <c r="F39" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="G39" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B40" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C40" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D40" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E40" t="s">
         <v>8</v>
       </c>
       <c r="F40" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="G40" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B41" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C41" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D41" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E41" t="s">
         <v>8</v>
       </c>
       <c r="F41" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="G41" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B42" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C42" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D42" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E42" t="s">
         <v>8</v>
       </c>
       <c r="F42" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="G42" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B43" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C43" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D43" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E43" t="s">
         <v>8</v>
@@ -1682,21 +1679,21 @@
         <v>8</v>
       </c>
       <c r="G43" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B44" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C44" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D44" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E44" t="s">
         <v>8</v>
@@ -1705,21 +1702,21 @@
         <v>8</v>
       </c>
       <c r="G44" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B45" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C45" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D45" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E45" t="s">
         <v>8</v>
@@ -1728,455 +1725,455 @@
         <v>8</v>
       </c>
       <c r="G45" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B46" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C46" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D46" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E46" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="F46" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G46" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
+        <v>15</v>
+      </c>
+      <c r="B47" t="s">
+        <v>16</v>
+      </c>
+      <c r="C47" t="s">
+        <v>24</v>
+      </c>
+      <c r="D47" t="s">
+        <v>23</v>
+      </c>
+      <c r="E47" t="s">
+        <v>21</v>
+      </c>
+      <c r="F47" t="s">
+        <v>23</v>
+      </c>
+      <c r="G47" t="s">
         <v>18</v>
-      </c>
-      <c r="B47" t="s">
-        <v>19</v>
-      </c>
-      <c r="C47" t="s">
-        <v>27</v>
-      </c>
-      <c r="D47" t="s">
-        <v>26</v>
-      </c>
-      <c r="E47" t="s">
-        <v>24</v>
-      </c>
-      <c r="F47" t="s">
-        <v>26</v>
-      </c>
-      <c r="G47" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B48" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C48" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D48" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E48" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F48" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G48" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B49" t="s">
+        <v>16</v>
+      </c>
+      <c r="C49" t="s">
+        <v>24</v>
+      </c>
+      <c r="D49" t="s">
+        <v>23</v>
+      </c>
+      <c r="E49" t="s">
+        <v>12</v>
+      </c>
+      <c r="F49" t="s">
+        <v>23</v>
+      </c>
+      <c r="G49" t="s">
         <v>19</v>
-      </c>
-      <c r="C49" t="s">
-        <v>27</v>
-      </c>
-      <c r="D49" t="s">
-        <v>26</v>
-      </c>
-      <c r="E49" t="s">
-        <v>15</v>
-      </c>
-      <c r="F49" t="s">
-        <v>26</v>
-      </c>
-      <c r="G49" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B50" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C50" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D50" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E50" t="s">
         <v>9</v>
       </c>
       <c r="F50" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G50" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B51" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C51" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D51" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E51" t="s">
         <v>9</v>
       </c>
       <c r="F51" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G51" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B52" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C52" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D52" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E52" t="s">
         <v>8</v>
       </c>
       <c r="F52" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G52" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B53" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C53" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D53" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E53" t="s">
         <v>8</v>
       </c>
       <c r="F53" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G53" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B54" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C54" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D54" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E54" t="s">
         <v>8</v>
       </c>
       <c r="F54" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G54" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B55" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C55" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D55" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E55" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="F55" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G55" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B56" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C56" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D56" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E56" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F56" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G56" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B57" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C57" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D57" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E57" t="s">
         <v>9</v>
       </c>
       <c r="F57" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G57" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B58" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C58" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D58" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E58" t="s">
         <v>8</v>
       </c>
       <c r="F58" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G58" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B59" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C59" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D59" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E59" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="F59" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G59" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
+        <v>16</v>
+      </c>
+      <c r="B60" t="s">
+        <v>16</v>
+      </c>
+      <c r="C60" t="s">
+        <v>24</v>
+      </c>
+      <c r="D60" t="s">
+        <v>33</v>
+      </c>
+      <c r="E60" t="s">
+        <v>12</v>
+      </c>
+      <c r="F60" t="s">
+        <v>23</v>
+      </c>
+      <c r="G60" t="s">
         <v>19</v>
-      </c>
-      <c r="B60" t="s">
-        <v>19</v>
-      </c>
-      <c r="C60" t="s">
-        <v>27</v>
-      </c>
-      <c r="D60" t="s">
-        <v>36</v>
-      </c>
-      <c r="E60" t="s">
-        <v>15</v>
-      </c>
-      <c r="F60" t="s">
-        <v>26</v>
-      </c>
-      <c r="G60" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B61" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C61" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D61" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E61" t="s">
         <v>9</v>
       </c>
       <c r="F61" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G61" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B62" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C62" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D62" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E62" t="s">
         <v>8</v>
       </c>
       <c r="F62" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G62" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B63" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C63" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D63" t="s">
         <v>10</v>
       </c>
       <c r="E63" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="F63" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G63" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B64" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C64" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D64" t="s">
         <v>10</v>
       </c>
       <c r="E64" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F64" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G64" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B65" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C65" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D65" t="s">
         <v>10</v>
@@ -2185,21 +2182,21 @@
         <v>9</v>
       </c>
       <c r="F65" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G65" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B66" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C66" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D66" t="s">
         <v>10</v>
@@ -2208,67 +2205,67 @@
         <v>8</v>
       </c>
       <c r="F66" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G66" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B67" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C67" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D67" t="s">
         <v>8</v>
       </c>
       <c r="E67" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="F67" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G67" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B68" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C68" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D68" t="s">
         <v>8</v>
       </c>
       <c r="E68" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F68" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G68" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B69" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C69" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D69" t="s">
         <v>8</v>
@@ -2277,21 +2274,21 @@
         <v>9</v>
       </c>
       <c r="F69" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G69" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B70" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C70" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D70" t="s">
         <v>8</v>
@@ -2300,286 +2297,286 @@
         <v>8</v>
       </c>
       <c r="F70" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G70" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
+        <v>16</v>
+      </c>
+      <c r="B71" t="s">
+        <v>16</v>
+      </c>
+      <c r="C71" t="s">
+        <v>25</v>
+      </c>
+      <c r="D71" t="s">
+        <v>23</v>
+      </c>
+      <c r="E71" t="s">
+        <v>23</v>
+      </c>
+      <c r="F71" t="s">
+        <v>23</v>
+      </c>
+      <c r="G71" t="s">
         <v>19</v>
-      </c>
-      <c r="B71" t="s">
-        <v>19</v>
-      </c>
-      <c r="C71" t="s">
-        <v>28</v>
-      </c>
-      <c r="D71" t="s">
-        <v>26</v>
-      </c>
-      <c r="E71" t="s">
-        <v>26</v>
-      </c>
-      <c r="F71" t="s">
-        <v>26</v>
-      </c>
-      <c r="G71" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B72" t="s">
+        <v>16</v>
+      </c>
+      <c r="C72" t="s">
+        <v>25</v>
+      </c>
+      <c r="D72" t="s">
+        <v>23</v>
+      </c>
+      <c r="E72" t="s">
+        <v>23</v>
+      </c>
+      <c r="F72" t="s">
+        <v>23</v>
+      </c>
+      <c r="G72" t="s">
         <v>19</v>
-      </c>
-      <c r="C72" t="s">
-        <v>28</v>
-      </c>
-      <c r="D72" t="s">
-        <v>26</v>
-      </c>
-      <c r="E72" t="s">
-        <v>26</v>
-      </c>
-      <c r="F72" t="s">
-        <v>26</v>
-      </c>
-      <c r="G72" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B73" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C73" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D73" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E73" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="F73" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G73" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
+        <v>16</v>
+      </c>
+      <c r="B74" t="s">
+        <v>15</v>
+      </c>
+      <c r="C74" t="s">
+        <v>25</v>
+      </c>
+      <c r="D74" t="s">
+        <v>23</v>
+      </c>
+      <c r="E74" t="s">
+        <v>12</v>
+      </c>
+      <c r="F74" t="s">
+        <v>23</v>
+      </c>
+      <c r="G74" t="s">
         <v>19</v>
-      </c>
-      <c r="B74" t="s">
-        <v>18</v>
-      </c>
-      <c r="C74" t="s">
-        <v>28</v>
-      </c>
-      <c r="D74" t="s">
-        <v>26</v>
-      </c>
-      <c r="E74" t="s">
-        <v>15</v>
-      </c>
-      <c r="F74" t="s">
-        <v>26</v>
-      </c>
-      <c r="G74" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B75" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C75" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D75" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E75" t="s">
         <v>9</v>
       </c>
       <c r="F75" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G75" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B76" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C76" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D76" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E76" t="s">
         <v>8</v>
       </c>
       <c r="F76" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G76" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B77" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C77" t="s">
         <v>8</v>
       </c>
       <c r="D77" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E77" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F77" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G77" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B78" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C78" t="s">
         <v>8</v>
       </c>
       <c r="D78" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E78" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F78" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G78" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B79" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C79" t="s">
         <v>8</v>
       </c>
       <c r="D79" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E79" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="F79" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G79" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B80" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C80" t="s">
         <v>8</v>
       </c>
       <c r="D80" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E80" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F80" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G80" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B81" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C81" t="s">
         <v>8</v>
       </c>
       <c r="D81" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E81" t="s">
         <v>9</v>
       </c>
       <c r="F81" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G81" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B82" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C82" t="s">
         <v>8</v>
       </c>
       <c r="D82" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E82" t="s">
         <v>8</v>
       </c>
       <c r="F82" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G82" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -2629,10 +2626,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="B1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -2644,27 +2641,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{049D8219-61F7-4CA8-8A64-D28D15908D92}">
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection sqref="A1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>13</v>
+        <v>45</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>12</v>
+        <v>46</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>14</v>
+        <v>47</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>11</v>
@@ -2678,7 +2675,7 @@
         <v>8</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>8</v>
@@ -2692,10 +2689,10 @@
         <v>1</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -2723,7 +2720,7 @@
         <v>5</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -2737,7 +2734,7 @@
         <v>4</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -2745,13 +2742,13 @@
         <v>6</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -2779,7 +2776,7 @@
         <v>5</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -2804,10 +2801,10 @@
         <v>1</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -2835,7 +2832,7 @@
         <v>5</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -2849,7 +2846,7 @@
         <v>4</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -2867,7 +2864,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCFCADA8-35EC-4674-BB10-19E37C561E05}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
@@ -2881,57 +2878,57 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>2</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>3</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Meetresultaat doet het nu ook
</commit_message>
<xml_diff>
--- a/src/main/resources/nhs-dmn/CHgestript.xlsx
+++ b/src/main/resources/nhs-dmn/CHgestript.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-20.04\home\han\git\rivm\nhs\dmn\nhs-business\src\main\resources\nhs-dmn\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3404C5F6-3EEC-49A7-8603-BBF84A7BF3DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDEC055F-C3AA-4D2D-B4F3-B5B9A87CAC8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="36975" yWindow="4650" windowWidth="28800" windowHeight="11295" tabRatio="834" activeTab="2" xr2:uid="{4203C9A5-FA6C-4E14-8325-EE7186AD0D41}"/>
+    <workbookView xWindow="28680" yWindow="-2235" windowWidth="38640" windowHeight="15720" tabRatio="834" xr2:uid="{4203C9A5-FA6C-4E14-8325-EE7186AD0D41}"/>
   </bookViews>
   <sheets>
     <sheet name="MeetResultaat" sheetId="22" r:id="rId1"/>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="647" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="647" uniqueCount="47">
   <si>
     <t>&lt;= 252</t>
   </si>
@@ -159,36 +159,6 @@
     <t>(40 .. 105]</t>
   </si>
   <si>
-    <t>hps.isPrematuur</t>
-  </si>
-  <si>
-    <t>hps.THP</t>
-  </si>
-  <si>
-    <t>hps.T4</t>
-  </si>
-  <si>
-    <t>hps.TBG</t>
-  </si>
-  <si>
-    <t>hps.TSH</t>
-  </si>
-  <si>
-    <t>hps."T4/TBG"</t>
-  </si>
-  <si>
-    <t>hps.hielprik.hielprikType</t>
-  </si>
-  <si>
-    <t>hps.redenOnbekend(hps.hielprik,"TSH")</t>
-  </si>
-  <si>
-    <t>hps.redenOnbekend(hps.hielprik,"T4/TBG")</t>
-  </si>
-  <si>
-    <t>hps.redenOnbekend(hps.hielprik,"T4")</t>
-  </si>
-  <si>
     <t>HPS.AfnametermijnPrematuur</t>
   </si>
   <si>
@@ -196,6 +166,33 @@
   </si>
   <si>
     <t>HPS.Geboortegewicht</t>
+  </si>
+  <si>
+    <t>HPS.T4</t>
+  </si>
+  <si>
+    <t>HPS.TBG</t>
+  </si>
+  <si>
+    <t>HPS.TSH</t>
+  </si>
+  <si>
+    <t>HPS.hielprik.hielprikType</t>
+  </si>
+  <si>
+    <t>HPS.bruikbaarheid(HPS.hielprik,"TSH")</t>
+  </si>
+  <si>
+    <t>HPS.bruikbaarheid(HPS.hielprik,"T4/TBG")</t>
+  </si>
+  <si>
+    <t>HPS.bruikbaarheid(HPS.hielprik,"T4")</t>
+  </si>
+  <si>
+    <t>isTweedeHielprik</t>
+  </si>
+  <si>
+    <t>HPS.T4_TBG</t>
   </si>
 </sst>
 </file>
@@ -677,9 +674,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{920955FF-C75C-492B-A53F-AFC4A746FDCE}">
   <dimension ref="A1:G82"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:G1048576"/>
+      <selection pane="bottomLeft" activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -695,22 +692,22 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>35</v>
+        <v>11</v>
       </c>
       <c r="B1" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="C1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F1" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="G1" t="s">
         <v>31</v>
@@ -2641,7 +2638,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{049D8219-61F7-4CA8-8A64-D28D15908D92}">
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection sqref="A1:D1048576"/>
     </sheetView>
   </sheetViews>
@@ -2655,13 +2652,13 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>11</v>

</xml_diff>

<commit_message>
isPrematuur nu direct vanaf hielprik
</commit_message>
<xml_diff>
--- a/src/main/resources/nhs-dmn/CHgestript.xlsx
+++ b/src/main/resources/nhs-dmn/CHgestript.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-20.04\home\han\git\rivm\nhs\dmn\nhs-business\src\main\resources\nhs-dmn\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E7D7079-D57F-4F8C-B603-D37DBAB96813}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD13106E-FDFC-4817-8104-0D61B11D0662}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-2235" windowWidth="38640" windowHeight="15720" tabRatio="834" xr2:uid="{4203C9A5-FA6C-4E14-8325-EE7186AD0D41}"/>
+    <workbookView xWindow="28680" yWindow="-2235" windowWidth="38640" windowHeight="15720" tabRatio="834" activeTab="2" xr2:uid="{4203C9A5-FA6C-4E14-8325-EE7186AD0D41}"/>
   </bookViews>
   <sheets>
     <sheet name="MeetResultaat" sheetId="22" r:id="rId1"/>
@@ -152,15 +152,6 @@
     <t>HPS.TSH</t>
   </si>
   <si>
-    <t>HPS.AfnametermijnPrematuur</t>
-  </si>
-  <si>
-    <t>HPS.Zwangerschapsduur</t>
-  </si>
-  <si>
-    <t>HPS.Geboortegewicht</t>
-  </si>
-  <si>
     <t>isTweedeHielprik</t>
   </si>
   <si>
@@ -180,6 +171,15 @@
   </si>
   <si>
     <t>HPS.classificatie(HPS.hielprik,"T4")</t>
+  </si>
+  <si>
+    <t>hielprik.afnametermijnPrematuur</t>
+  </si>
+  <si>
+    <t>hielprik.zwangerschapsduur</t>
+  </si>
+  <si>
+    <t>hielprik.geboortegewicht</t>
   </si>
 </sst>
 </file>
@@ -658,7 +658,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{920955FF-C75C-492B-A53F-AFC4A746FDCE}">
   <dimension ref="A1:G86"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="G5" sqref="G5"/>
     </sheetView>
@@ -679,7 +679,7 @@
         <v>9</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>30</v>
@@ -691,7 +691,7 @@
         <v>32</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>26</v>
@@ -786,7 +786,7 @@
         <v>23</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -1016,7 +1016,7 @@
         <v>23</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -1039,7 +1039,7 @@
         <v>23</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -1062,7 +1062,7 @@
         <v>23</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -1338,7 +1338,7 @@
         <v>6</v>
       </c>
       <c r="G29" s="4" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
@@ -1361,7 +1361,7 @@
         <v>6</v>
       </c>
       <c r="G30" s="4" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
@@ -1522,7 +1522,7 @@
         <v>11</v>
       </c>
       <c r="G37" s="4" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
@@ -1568,7 +1568,7 @@
         <v>11</v>
       </c>
       <c r="G39" s="4" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
@@ -1591,7 +1591,7 @@
         <v>11</v>
       </c>
       <c r="G40" s="4" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
@@ -1614,7 +1614,7 @@
         <v>11</v>
       </c>
       <c r="G41" s="4" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
@@ -1637,7 +1637,7 @@
         <v>11</v>
       </c>
       <c r="G42" s="4" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
@@ -1660,7 +1660,7 @@
         <v>6</v>
       </c>
       <c r="G43" s="4" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
@@ -1683,7 +1683,7 @@
         <v>6</v>
       </c>
       <c r="G44" s="4" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
@@ -1706,7 +1706,7 @@
         <v>6</v>
       </c>
       <c r="G45" s="4" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
@@ -1913,7 +1913,7 @@
         <v>23</v>
       </c>
       <c r="G54" s="4" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
@@ -2097,7 +2097,7 @@
         <v>23</v>
       </c>
       <c r="G62" s="4" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
@@ -2419,7 +2419,7 @@
         <v>23</v>
       </c>
       <c r="G76" s="4" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
@@ -2442,7 +2442,7 @@
         <v>23</v>
       </c>
       <c r="G77" s="4" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
@@ -2465,7 +2465,7 @@
         <v>23</v>
       </c>
       <c r="G78" s="4" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
@@ -2488,7 +2488,7 @@
         <v>23</v>
       </c>
       <c r="G79" s="4" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
@@ -2534,7 +2534,7 @@
         <v>23</v>
       </c>
       <c r="G81" s="4" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
@@ -2557,7 +2557,7 @@
         <v>23</v>
       </c>
       <c r="G82" s="4" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
@@ -2647,7 +2647,7 @@
         <v>29</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -2660,7 +2660,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>14</v>
@@ -2676,7 +2676,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>13</v>
@@ -2691,8 +2691,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{049D8219-61F7-4CA8-8A64-D28D15908D92}">
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:D2"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2705,13 +2705,13 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
Origineel weer gestript en geintegreerd
</commit_message>
<xml_diff>
--- a/src/main/resources/nhs-dmn/CHgestript.xlsx
+++ b/src/main/resources/nhs-dmn/CHgestript.xlsx
@@ -8,18 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-20.04\home\han\git\rivm\nhs\dmn\nhs-business\src\main\resources\nhs-dmn\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD13106E-FDFC-4817-8104-0D61B11D0662}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B8EFAC6-B4B8-4F84-9C50-5CC222094372}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-2235" windowWidth="38640" windowHeight="15720" tabRatio="834" activeTab="2" xr2:uid="{4203C9A5-FA6C-4E14-8325-EE7186AD0D41}"/>
   </bookViews>
   <sheets>
-    <sheet name="MeetResultaat" sheetId="22" r:id="rId1"/>
+    <sheet name="Interpretatie" sheetId="22" r:id="rId1"/>
     <sheet name="isTweedeHielprik" sheetId="24" r:id="rId2"/>
     <sheet name="isPrematuur" sheetId="13" r:id="rId3"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Interpretatie!$A$1:$G$77</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">isPrematuur!$A$1:$D$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">MeetResultaat!$A$1:$G$82</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">isTweedeHielprik!$A$1:$B$1</definedName>
     <definedName name="AfnameTermijnVeld">#REF!</definedName>
     <definedName name="ClassificatieVeld">#REF!</definedName>
     <definedName name="HielprikTypeVeld">#REF!</definedName>
@@ -51,7 +52,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="640" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="605" uniqueCount="43">
+  <si>
+    <t>Interpretatie</t>
+  </si>
   <si>
     <t>&lt;= 252</t>
   </si>
@@ -131,9 +135,6 @@
     <t>&gt; -0.8</t>
   </si>
   <si>
-    <t>MeetResultaat</t>
-  </si>
-  <si>
     <t>&lt;= 40</t>
   </si>
   <si>
@@ -164,13 +165,13 @@
     <t>HPS.T4_TBG</t>
   </si>
   <si>
+    <t>HPS.classificatie(HPS.hielprik,"T4")</t>
+  </si>
+  <si>
     <t>HPS.classificatie(HPS.hielprik,"TSH")</t>
   </si>
   <si>
     <t>HPS.classificatie(HPS.hielprik,"T4/TBG")</t>
-  </si>
-  <si>
-    <t>HPS.classificatie(HPS.hielprik,"T4")</t>
   </si>
   <si>
     <t>hielprik.afnametermijnPrematuur</t>
@@ -656,11 +657,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{920955FF-C75C-492B-A53F-AFC4A746FDCE}">
-  <dimension ref="A1:G86"/>
+  <dimension ref="A1:G80"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G5" sqref="G5"/>
+      <selection pane="bottomLeft" activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -676,7 +677,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>33</v>
@@ -694,165 +695,165 @@
         <v>36</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>26</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C6" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>21</v>
-      </c>
       <c r="F6" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C7" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D7" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>21</v>
-      </c>
       <c r="F7" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>14</v>
       </c>
       <c r="C8" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D8" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>21</v>
-      </c>
       <c r="F8" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G8" s="4" t="s">
         <v>18</v>
@@ -863,19 +864,19 @@
         <v>14</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C9" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E9" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D9" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>10</v>
-      </c>
       <c r="F9" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G9" s="4" t="s">
         <v>19</v>
@@ -883,71 +884,71 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>14</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>14</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -955,183 +956,183 @@
         <v>14</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>14</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>37</v>
+        <v>18</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>37</v>
+        <v>18</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>37</v>
+        <v>18</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>18</v>
+        <v>38</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>14</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>18</v>
+        <v>38</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>17</v>
+        <v>38</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -1139,68 +1140,68 @@
         <v>14</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>17</v>
+        <v>38</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="G22" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="G23" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -1208,137 +1209,137 @@
         <v>14</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>14</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G25" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>14</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G26" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B27" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F27" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C27" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E27" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F27" s="3" t="s">
-        <v>12</v>
-      </c>
       <c r="G27" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>14</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="G28" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>14</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G29" s="4" t="s">
-        <v>38</v>
+        <v>18</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
@@ -1346,42 +1347,42 @@
         <v>14</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C30" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F30" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G30" s="4" t="s">
         <v>20</v>
-      </c>
-      <c r="D30" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E30" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F30" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="G30" s="4" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="G31" s="4" t="s">
         <v>19</v>
@@ -1389,140 +1390,140 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>14</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="G32" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F33" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B33" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C33" s="3" t="s">
+      <c r="G33" s="4" t="s">
         <v>20</v>
-      </c>
-      <c r="D33" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E33" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F33" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="G33" s="4" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B34" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F34" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C34" s="3" t="s">
+      <c r="G34" s="4" t="s">
         <v>20</v>
-      </c>
-      <c r="D34" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E34" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F34" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G34" s="4" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="G35" s="4" t="s">
-        <v>17</v>
+        <v>39</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G36" s="4" t="s">
-        <v>17</v>
+        <v>39</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="G37" s="4" t="s">
-        <v>37</v>
+        <v>18</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
@@ -1530,183 +1531,183 @@
         <v>14</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="G38" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E39" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F39" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B39" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C39" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D39" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E39" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F39" s="3" t="s">
-        <v>11</v>
-      </c>
       <c r="G39" s="4" t="s">
-        <v>37</v>
+        <v>18</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B40" s="3" t="s">
         <v>14</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="G40" s="4" t="s">
-        <v>37</v>
+        <v>18</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F41" s="3" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="G41" s="4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F42" s="3" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="G42" s="4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B43" s="3" t="s">
         <v>14</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F43" s="3" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="G43" s="4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F44" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G44" s="4" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B45" s="3" t="s">
         <v>14</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="F45" s="3" t="s">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="G45" s="4" t="s">
-        <v>37</v>
+        <v>18</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
@@ -1714,45 +1715,45 @@
         <v>14</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F46" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G46" s="4" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="F47" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G47" s="4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
@@ -1760,272 +1761,272 @@
         <v>14</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F48" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G48" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="F49" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G49" s="4" t="s">
-        <v>19</v>
+        <v>38</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="F50" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G50" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="F51" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G51" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F52" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G52" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="E53" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F53" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G53" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="E54" s="3" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="F54" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G54" s="4" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E55" s="3" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="F55" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G55" s="4" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E56" s="3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F56" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G56" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E57" s="3" t="s">
         <v>7</v>
       </c>
       <c r="F57" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G57" s="4" t="s">
-        <v>17</v>
+        <v>38</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="E58" s="3" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="F58" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G58" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>27</v>
+        <v>9</v>
       </c>
       <c r="E59" s="3" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="F59" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G59" s="4" t="s">
         <v>18</v>
@@ -2033,163 +2034,163 @@
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>27</v>
+        <v>9</v>
       </c>
       <c r="E60" s="3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F60" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G60" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>27</v>
+        <v>9</v>
       </c>
       <c r="E61" s="3" t="s">
         <v>7</v>
       </c>
       <c r="F61" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G61" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>27</v>
+        <v>7</v>
       </c>
       <c r="E62" s="3" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="F62" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G62" s="4" t="s">
-        <v>37</v>
+        <v>18</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E63" s="3" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="F63" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G63" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D64" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E64" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E64" s="3" t="s">
-        <v>10</v>
-      </c>
       <c r="F64" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G64" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E65" s="3" t="s">
         <v>7</v>
       </c>
       <c r="F65" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G65" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="E66" s="3" t="s">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="F66" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G66" s="4" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
@@ -2197,137 +2198,137 @@
         <v>14</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D67" s="3" t="s">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="E67" s="3" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="F67" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G67" s="4" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B68" s="3" t="s">
         <v>14</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D68" s="3" t="s">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="E68" s="3" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="F68" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G68" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B69" s="3" t="s">
         <v>14</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D69" s="3" t="s">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="E69" s="3" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="F69" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G69" s="4" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B70" s="3" t="s">
         <v>14</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D70" s="3" t="s">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="E70" s="3" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F70" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G70" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B71" s="3" t="s">
         <v>14</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D71" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E71" s="3" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="F71" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G71" s="4" t="s">
-        <v>19</v>
+        <v>38</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" s="3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="D72" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E72" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F72" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G72" s="4" t="s">
-        <v>19</v>
+        <v>37</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
@@ -2335,88 +2336,88 @@
         <v>14</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="D73" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E73" s="3" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="F73" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G73" s="4" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C74" s="3" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="D74" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E74" s="3" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="F74" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G74" s="4" t="s">
-        <v>19</v>
+        <v>37</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C75" s="3" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="D75" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E75" s="3" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="F75" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G75" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C76" s="3" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="D76" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E76" s="3" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F76" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G76" s="4" t="s">
         <v>37</v>
@@ -2424,187 +2425,71 @@
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B77" s="3" t="s">
         <v>14</v>
       </c>
       <c r="C77" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D77" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E77" s="3" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="F77" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G77" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A78" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B78" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C78" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D78" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E78" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="F78" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="G78" s="4" t="s">
-        <v>39</v>
-      </c>
+      <c r="A78" s="3"/>
+      <c r="B78" s="3"/>
+      <c r="C78" s="3"/>
+      <c r="D78" s="3"/>
+      <c r="E78" s="3"/>
+      <c r="F78" s="3"/>
+      <c r="G78" s="4"/>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A79" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B79" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C79" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D79" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E79" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="F79" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="G79" s="4" t="s">
-        <v>39</v>
-      </c>
+      <c r="A79" s="3"/>
+      <c r="B79" s="3"/>
+      <c r="C79" s="3"/>
+      <c r="D79" s="3"/>
+      <c r="E79" s="3"/>
+      <c r="F79" s="3"/>
+      <c r="G79" s="4"/>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A80" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B80" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C80" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D80" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E80" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F80" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="G80" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A81" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B81" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C81" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D81" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E81" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F81" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="G81" s="4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A82" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B82" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C82" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D82" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E82" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F82" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="G82" s="4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A83" s="3"/>
-      <c r="B83" s="3"/>
-      <c r="C83" s="3"/>
-      <c r="D83" s="3"/>
-      <c r="E83" s="3"/>
-      <c r="F83" s="3"/>
-      <c r="G83" s="4"/>
-    </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A84" s="3"/>
-      <c r="B84" s="3"/>
-      <c r="C84" s="3"/>
-      <c r="D84" s="3"/>
-      <c r="E84" s="3"/>
-      <c r="F84" s="3"/>
-      <c r="G84" s="4"/>
-    </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A85" s="3"/>
-      <c r="B85" s="3"/>
-      <c r="C85" s="3"/>
-      <c r="D85" s="3"/>
-      <c r="E85" s="3"/>
-      <c r="F85" s="3"/>
-      <c r="G85" s="4"/>
-    </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A86" s="3"/>
-      <c r="B86" s="3"/>
-      <c r="C86" s="3"/>
-      <c r="D86" s="3"/>
-      <c r="E86" s="3"/>
-      <c r="F86" s="3"/>
-      <c r="G86" s="4"/>
+      <c r="A80" s="3"/>
+      <c r="B80" s="3"/>
+      <c r="C80" s="3"/>
+      <c r="D80" s="3"/>
+      <c r="E80" s="3"/>
+      <c r="F80" s="3"/>
+      <c r="G80" s="4"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G82" xr:uid="{920955FF-C75C-492B-A53F-AFC4A746FDCE}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G65">
-    <sortCondition ref="E2:E65"/>
-    <sortCondition ref="C2:C65"/>
-    <sortCondition ref="D2:D65"/>
-    <sortCondition ref="B2:B65"/>
+  <autoFilter ref="A1:G77" xr:uid="{920955FF-C75C-492B-A53F-AFC4A746FDCE}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G80">
+    <sortCondition ref="C2:C80"/>
+    <sortCondition ref="D2:D80"/>
+    <sortCondition ref="E2:E80"/>
+    <sortCondition ref="F2:F80"/>
+    <sortCondition ref="A2:A80"/>
+    <sortCondition ref="B2:B80"/>
   </sortState>
   <dataValidations count="6">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F74:F1048576 F68 F71 F2:F65" xr:uid="{D98EEB01-15FD-4F82-BF5B-19D9CD4CB583}">
+      <formula1>T4_TBG</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F72:F73 F66:F67 F69:F70 D2:D1048576" xr:uid="{69C6B805-FC6D-42F8-BE78-74C15213AAA0}">
+      <formula1>TBG_Waarden</formula1>
+    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G1048576" xr:uid="{931C25AC-710B-4B8F-82FC-202F8C5B3ED0}">
       <formula1>MeetResultaat</formula1>
     </dataValidation>
@@ -2613,12 +2498,6 @@
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C1048576" xr:uid="{FFF7110F-C8B6-40B7-B363-DA6A08EBA356}">
       <formula1>T4_Waarden</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F79:F1048576 F73 F76 F2:F70" xr:uid="{D98EEB01-15FD-4F82-BF5B-19D9CD4CB583}">
-      <formula1>T4_TBG</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F77:F78 F71:F72 F74:F75 D2:D1048576" xr:uid="{69C6B805-FC6D-42F8-BE78-74C15213AAA0}">
-      <formula1>TBG_Waarden</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E1048576" xr:uid="{B79108E4-5357-406A-91F1-FE388C00E150}">
       <formula1>TSH_Waarden</formula1>
@@ -2633,7 +2512,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:B5"/>
+      <selection sqref="A1:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2652,10 +2531,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -2663,15 +2542,15 @@
         <v>34</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -2679,10 +2558,11 @@
         <v>35</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:B1" xr:uid="{BC7F772D-6CFE-4AB8-B0B9-51B0606D75BB}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2691,15 +2571,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{049D8219-61F7-4CA8-8A64-D28D15908D92}">
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2714,189 +2594,189 @@
         <v>42</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Synchronisatie en kleine oneffenheden weggewerkt
</commit_message>
<xml_diff>
--- a/src/main/resources/nhs-dmn/CHgestript.xlsx
+++ b/src/main/resources/nhs-dmn/CHgestript.xlsx
@@ -8,24 +8,30 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-20.04\home\han\git\rivm\nhs\dmn\nhs-business\src\main\resources\nhs-dmn\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B8EFAC6-B4B8-4F84-9C50-5CC222094372}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6479D7F-FC38-4C29-AECB-A29F8147F4F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-2235" windowWidth="38640" windowHeight="15720" tabRatio="834" activeTab="2" xr2:uid="{4203C9A5-FA6C-4E14-8325-EE7186AD0D41}"/>
+    <workbookView xWindow="37035" yWindow="-435" windowWidth="28335" windowHeight="11295" tabRatio="834" activeTab="4" xr2:uid="{4203C9A5-FA6C-4E14-8325-EE7186AD0D41}"/>
   </bookViews>
   <sheets>
-    <sheet name="Interpretatie" sheetId="22" r:id="rId1"/>
-    <sheet name="isTweedeHielprik" sheetId="24" r:id="rId2"/>
-    <sheet name="isPrematuur" sheetId="13" r:id="rId3"/>
+    <sheet name="Actiecode" sheetId="10" r:id="rId1"/>
+    <sheet name="BTnavraagNodig" sheetId="15" r:id="rId2"/>
+    <sheet name="Interpretatie" sheetId="22" r:id="rId3"/>
+    <sheet name="isTweedeHielprik" sheetId="24" r:id="rId4"/>
+    <sheet name="isPrematuur" sheetId="13" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Interpretatie!$A$1:$G$77</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">isPrematuur!$A$1:$D$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">isTweedeHielprik!$A$1:$B$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">BTnavraagNodig!$A$1:$D$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Interpretatie!$A$1:$G$77</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">isPrematuur!$A$1:$D$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">isTweedeHielprik!$A$1:$B$1</definedName>
     <definedName name="AfnameTermijnVeld">#REF!</definedName>
+    <definedName name="BloedTransfusieType">#REF!</definedName>
     <definedName name="ClassificatieVeld">#REF!</definedName>
+    <definedName name="Erytrocyten">#REF!</definedName>
     <definedName name="HielprikTypeVeld">#REF!</definedName>
     <definedName name="Interpretatie">#REF!</definedName>
     <definedName name="JaNeeVeld">#REF!</definedName>
+    <definedName name="leegNietleeg">#REF!</definedName>
     <definedName name="MeetResultaat">#REF!</definedName>
     <definedName name="T4_TBG">#REF!</definedName>
     <definedName name="T4_Waarden">#REF!</definedName>
@@ -52,7 +58,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="605" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="686" uniqueCount="67">
+  <si>
+    <t>Actiecode</t>
+  </si>
   <si>
     <t>Interpretatie</t>
   </si>
@@ -117,6 +126,12 @@
     <t>"Negatief"</t>
   </si>
   <si>
+    <t>"NIET CLASSIFICEERBAAR"</t>
+  </si>
+  <si>
+    <t>"NIET UITGEVOERD"</t>
+  </si>
+  <si>
     <t>(-3.0 .. -1.6]</t>
   </si>
   <si>
@@ -181,6 +196,69 @@
   </si>
   <si>
     <t>hielprik.geboortegewicht</t>
+  </si>
+  <si>
+    <t>hielprik.bloedtransfusie</t>
+  </si>
+  <si>
+    <t>hielprik.bloedtransfusieMoment</t>
+  </si>
+  <si>
+    <t>hielprik.bloedtransfusieType</t>
+  </si>
+  <si>
+    <t>not(null)</t>
+  </si>
+  <si>
+    <t>"Erytrocyten"</t>
+  </si>
+  <si>
+    <t>"Trombocyten"</t>
+  </si>
+  <si>
+    <t>"Bloedplasma"</t>
+  </si>
+  <si>
+    <t>"Gemigreerd"</t>
+  </si>
+  <si>
+    <t>"Onbekend bij screener"</t>
+  </si>
+  <si>
+    <t>"Selecteer een type"</t>
+  </si>
+  <si>
+    <t>"Niet van toepassing"</t>
+  </si>
+  <si>
+    <t>HPS.isTeVroegGeprikt</t>
+  </si>
+  <si>
+    <t>BTnavraagNodig</t>
+  </si>
+  <si>
+    <t>"AFW"</t>
+  </si>
+  <si>
+    <t>"DUB"</t>
+  </si>
+  <si>
+    <t>"EHPTVG"</t>
+  </si>
+  <si>
+    <t>"BTF"</t>
+  </si>
+  <si>
+    <t>"ACTIENR4</t>
+  </si>
+  <si>
+    <t>"ACTIENR7</t>
+  </si>
+  <si>
+    <t>"GEENIRL</t>
+  </si>
+  <si>
+    <t>"GEENACTIE"</t>
   </si>
 </sst>
 </file>
@@ -321,7 +399,7 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -330,6 +408,9 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="3" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="4" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -656,12 +737,453 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{510755D5-C225-4368-836B-774EA8447DE4}">
+  <dimension ref="A1:D17"/>
+  <sheetViews>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18" customWidth="1"/>
+    <col min="3" max="3" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="4"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="3"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="4"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="3"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="4"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="3"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="4"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="3"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="4"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="3"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="4"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="3"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="4"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="3"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="4"/>
+    </row>
+  </sheetData>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A1048576" xr:uid="{5CEB2CE4-8CFA-4134-81D2-BFB2D7298F51}">
+      <formula1>Interpretatie</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:C1048576" xr:uid="{B7860D93-30E1-4DF2-B242-9FCAB1ADD29B}">
+      <formula1>JaNeeVeld</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B88B274-76A9-4F9C-97E3-D90602F3F1BF}">
+  <dimension ref="A1:F17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="3"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="4"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="3"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="4"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="3"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="4"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="3"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="4"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="3"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="4"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="3"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="4"/>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:D1" xr:uid="{3B88B274-76A9-4F9C-97E3-D90602F3F1BF}"/>
+  <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576 A2:A1048576" xr:uid="{75E19434-2472-400E-B76E-3ADE4D91B52D}">
+      <formula1>JaNeeVeld</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B1048576" xr:uid="{258920BA-B169-42AD-8FAE-49B3AE3EA323}">
+      <formula1>leegNietleeg</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C1048576" xr:uid="{E3764C45-08E2-49E2-9D7A-18795AE11294}">
+      <formula1>BloedTransfusieType</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{BD0A0A67-4B76-4854-88BC-63422455BFAE}">
+          <x14:formula1>
+            <xm:f>#REF!</xm:f>
+          </x14:formula1>
+          <xm:sqref>B1</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{920955FF-C75C-492B-A53F-AFC4A746FDCE}">
   <dimension ref="A1:G80"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J23" sqref="J23"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H1" sqref="H1:I1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -677,1773 +1199,1773 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="D1" s="1" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>18</v>
+        <v>27</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>20</v>
+        <v>27</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>18</v>
+        <v>27</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>38</v>
+        <v>27</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>19</v>
+        <v>27</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>18</v>
+        <v>27</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="G8" s="4" t="s">
-        <v>18</v>
+        <v>27</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="G9" s="4" t="s">
-        <v>19</v>
+        <v>27</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="G10" s="4" t="s">
-        <v>20</v>
+        <v>27</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="G11" s="4" t="s">
-        <v>20</v>
+        <v>27</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="G12" s="4" t="s">
-        <v>20</v>
+        <v>27</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="G13" s="4" t="s">
-        <v>20</v>
+        <v>27</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="G14" s="4" t="s">
-        <v>18</v>
+        <v>27</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="G15" s="4" t="s">
-        <v>18</v>
+        <v>27</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="G16" s="4" t="s">
-        <v>18</v>
+        <v>27</v>
+      </c>
+      <c r="G16" s="5" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="G17" s="4" t="s">
-        <v>18</v>
+        <v>27</v>
+      </c>
+      <c r="G17" s="5" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="G18" s="4" t="s">
-        <v>38</v>
+        <v>27</v>
+      </c>
+      <c r="G18" s="5" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="G19" s="4" t="s">
-        <v>38</v>
+        <v>27</v>
+      </c>
+      <c r="G19" s="5" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="G20" s="4" t="s">
-        <v>38</v>
+        <v>27</v>
+      </c>
+      <c r="G20" s="5" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="G21" s="4" t="s">
-        <v>38</v>
+        <v>27</v>
+      </c>
+      <c r="G21" s="5" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G22" s="4" t="s">
-        <v>18</v>
+        <v>13</v>
+      </c>
+      <c r="G22" s="5" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="G23" s="4" t="s">
-        <v>19</v>
+        <v>27</v>
+      </c>
+      <c r="G23" s="5" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="G24" s="4" t="s">
-        <v>19</v>
+        <v>27</v>
+      </c>
+      <c r="G24" s="5" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G25" s="4" t="s">
-        <v>18</v>
+        <v>13</v>
+      </c>
+      <c r="G25" s="5" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B26" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F26" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C26" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E26" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="F26" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G26" s="4" t="s">
-        <v>18</v>
+      <c r="G26" s="5" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B27" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F27" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C27" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E27" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="F27" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G27" s="4" t="s">
-        <v>18</v>
+      <c r="G27" s="5" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="G28" s="4" t="s">
-        <v>18</v>
+        <v>8</v>
+      </c>
+      <c r="G28" s="5" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="G29" s="4" t="s">
-        <v>18</v>
+        <v>8</v>
+      </c>
+      <c r="G29" s="5" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C30" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F30" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G30" s="5" t="s">
         <v>21</v>
-      </c>
-      <c r="D30" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E30" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F30" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="G30" s="4" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G31" s="4" t="s">
-        <v>19</v>
+        <v>13</v>
+      </c>
+      <c r="G31" s="5" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G32" s="4" t="s">
-        <v>18</v>
+        <v>13</v>
+      </c>
+      <c r="G32" s="5" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C33" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F33" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G33" s="5" t="s">
         <v>21</v>
-      </c>
-      <c r="D33" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E33" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F33" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G33" s="4" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B34" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F34" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C34" s="3" t="s">
+      <c r="G34" s="5" t="s">
         <v>21</v>
-      </c>
-      <c r="D34" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E34" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F34" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G34" s="4" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="G35" s="4" t="s">
-        <v>39</v>
+        <v>8</v>
+      </c>
+      <c r="G35" s="5" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="G36" s="4" t="s">
-        <v>39</v>
+        <v>8</v>
+      </c>
+      <c r="G36" s="5" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="G37" s="4" t="s">
-        <v>18</v>
+        <v>27</v>
+      </c>
+      <c r="G37" s="5" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="G38" s="4" t="s">
-        <v>18</v>
+        <v>27</v>
+      </c>
+      <c r="G38" s="5" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B39" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E39" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F39" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C39" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D39" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E39" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F39" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G39" s="4" t="s">
-        <v>18</v>
+      <c r="G39" s="5" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="G40" s="4" t="s">
-        <v>18</v>
+        <v>8</v>
+      </c>
+      <c r="G40" s="5" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F41" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="G41" s="4" t="s">
-        <v>38</v>
+        <v>27</v>
+      </c>
+      <c r="G41" s="5" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F42" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="G42" s="4" t="s">
-        <v>38</v>
+        <v>27</v>
+      </c>
+      <c r="G42" s="5" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B43" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E43" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F43" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C43" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D43" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E43" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F43" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G43" s="4" t="s">
-        <v>38</v>
+      <c r="G43" s="5" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F44" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="G44" s="4" t="s">
-        <v>39</v>
+        <v>8</v>
+      </c>
+      <c r="G44" s="5" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F45" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="G45" s="4" t="s">
-        <v>18</v>
+        <v>27</v>
+      </c>
+      <c r="G45" s="5" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C46" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D46" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E46" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D46" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E46" s="3" t="s">
-        <v>22</v>
-      </c>
       <c r="F46" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="G46" s="4" t="s">
-        <v>19</v>
+        <v>27</v>
+      </c>
+      <c r="G46" s="5" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F47" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="G47" s="4" t="s">
-        <v>20</v>
+        <v>27</v>
+      </c>
+      <c r="G47" s="5" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F48" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="G48" s="4" t="s">
-        <v>18</v>
+        <v>27</v>
+      </c>
+      <c r="G48" s="5" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F49" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="G49" s="4" t="s">
-        <v>38</v>
+        <v>27</v>
+      </c>
+      <c r="G49" s="5" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C50" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D50" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E50" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D50" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E50" s="3" t="s">
-        <v>22</v>
-      </c>
       <c r="F50" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="G50" s="4" t="s">
-        <v>18</v>
+        <v>27</v>
+      </c>
+      <c r="G50" s="5" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F51" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="G51" s="4" t="s">
-        <v>18</v>
+        <v>27</v>
+      </c>
+      <c r="G51" s="5" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F52" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="G52" s="4" t="s">
-        <v>18</v>
+        <v>27</v>
+      </c>
+      <c r="G52" s="5" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="E53" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F53" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="G53" s="4" t="s">
-        <v>18</v>
+        <v>27</v>
+      </c>
+      <c r="G53" s="5" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C54" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D54" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E54" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D54" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E54" s="3" t="s">
-        <v>22</v>
-      </c>
       <c r="F54" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="G54" s="4" t="s">
-        <v>19</v>
+        <v>27</v>
+      </c>
+      <c r="G54" s="5" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="E55" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F55" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="G55" s="4" t="s">
-        <v>20</v>
+        <v>27</v>
+      </c>
+      <c r="G55" s="5" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="E56" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F56" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="G56" s="4" t="s">
-        <v>18</v>
+        <v>27</v>
+      </c>
+      <c r="G56" s="5" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="E57" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F57" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="G57" s="4" t="s">
-        <v>38</v>
+        <v>27</v>
+      </c>
+      <c r="G57" s="5" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C58" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D58" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E58" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D58" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E58" s="3" t="s">
-        <v>22</v>
-      </c>
       <c r="F58" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="G58" s="4" t="s">
-        <v>18</v>
+        <v>27</v>
+      </c>
+      <c r="G58" s="5" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E59" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F59" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="G59" s="4" t="s">
-        <v>18</v>
+        <v>27</v>
+      </c>
+      <c r="G59" s="5" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="D60" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E60" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E60" s="3" t="s">
-        <v>8</v>
-      </c>
       <c r="F60" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="G60" s="4" t="s">
-        <v>18</v>
+        <v>27</v>
+      </c>
+      <c r="G60" s="5" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E61" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F61" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="G61" s="4" t="s">
-        <v>18</v>
+        <v>27</v>
+      </c>
+      <c r="G61" s="5" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C62" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D62" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E62" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D62" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E62" s="3" t="s">
-        <v>22</v>
-      </c>
       <c r="F62" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="G62" s="4" t="s">
-        <v>18</v>
+        <v>27</v>
+      </c>
+      <c r="G62" s="5" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E63" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F63" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="G63" s="4" t="s">
-        <v>18</v>
+        <v>27</v>
+      </c>
+      <c r="G63" s="5" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E64" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F64" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="G64" s="4" t="s">
-        <v>18</v>
+        <v>27</v>
+      </c>
+      <c r="G64" s="5" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E65" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F65" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="G65" s="4" t="s">
-        <v>18</v>
+        <v>27</v>
+      </c>
+      <c r="G65" s="5" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E66" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F66" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="G66" s="4" t="s">
-        <v>20</v>
+        <v>27</v>
+      </c>
+      <c r="G66" s="5" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="D67" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E67" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F67" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="G67" s="4" t="s">
-        <v>20</v>
+        <v>27</v>
+      </c>
+      <c r="G67" s="5" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="D68" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E68" s="3" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="F68" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="G68" s="4" t="s">
-        <v>18</v>
+        <v>27</v>
+      </c>
+      <c r="G68" s="5" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="D69" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E69" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F69" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="G69" s="4" t="s">
-        <v>20</v>
+        <v>27</v>
+      </c>
+      <c r="G69" s="5" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="D70" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E70" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F70" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="G70" s="4" t="s">
-        <v>18</v>
+        <v>27</v>
+      </c>
+      <c r="G70" s="5" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="D71" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E71" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F71" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="G71" s="4" t="s">
-        <v>38</v>
+        <v>27</v>
+      </c>
+      <c r="G71" s="5" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D72" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E72" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F72" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="G72" s="4" t="s">
-        <v>37</v>
+        <v>27</v>
+      </c>
+      <c r="G72" s="5" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D73" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E73" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F73" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="G73" s="4" t="s">
-        <v>37</v>
+        <v>27</v>
+      </c>
+      <c r="G73" s="5" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C74" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D74" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E74" s="3" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="F74" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="G74" s="4" t="s">
-        <v>37</v>
+        <v>27</v>
+      </c>
+      <c r="G74" s="5" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C75" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D75" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E75" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F75" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="G75" s="4" t="s">
-        <v>18</v>
+        <v>27</v>
+      </c>
+      <c r="G75" s="5" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C76" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D76" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E76" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F76" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="G76" s="4" t="s">
-        <v>37</v>
+        <v>27</v>
+      </c>
+      <c r="G76" s="5" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C77" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D77" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E77" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F77" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="G77" s="4" t="s">
-        <v>37</v>
+        <v>27</v>
+      </c>
+      <c r="G77" s="5" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
@@ -2453,7 +2975,7 @@
       <c r="D78" s="3"/>
       <c r="E78" s="3"/>
       <c r="F78" s="3"/>
-      <c r="G78" s="4"/>
+      <c r="G78" s="5"/>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" s="3"/>
@@ -2462,7 +2984,7 @@
       <c r="D79" s="3"/>
       <c r="E79" s="3"/>
       <c r="F79" s="3"/>
-      <c r="G79" s="4"/>
+      <c r="G79" s="5"/>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" s="3"/>
@@ -2471,7 +2993,7 @@
       <c r="D80" s="3"/>
       <c r="E80" s="3"/>
       <c r="F80" s="3"/>
-      <c r="G80" s="4"/>
+      <c r="G80" s="5"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:G77" xr:uid="{920955FF-C75C-492B-A53F-AFC4A746FDCE}"/>
@@ -2507,7 +3029,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC7F772D-6CFE-4AB8-B0B9-51B0606D75BB}">
   <dimension ref="A1:B5"/>
   <sheetViews>
@@ -2523,42 +3045,42 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>15</v>
+        <v>17</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>15</v>
+        <v>37</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>14</v>
+        <v>18</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>14</v>
+        <v>38</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -2567,11 +3089,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{049D8219-61F7-4CA8-8A64-D28D15908D92}">
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
@@ -2585,198 +3107,198 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>7</v>
+        <v>27</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>15</v>
+        <v>27</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>15</v>
+        <v>5</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>14</v>
+        <v>4</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>14</v>
+        <v>27</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>15</v>
+        <v>5</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>7</v>
+        <v>4</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>15</v>
+        <v>27</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>15</v>
+        <v>5</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>14</v>
+        <v>4</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>